<commit_message>
Allow bell initialization list Parameterize cache by container type. cons fix flatten sequence iterator from container list returns referrence documentation
</commit_message>
<xml_diff>
--- a/gop.xlsx
+++ b/gop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\tmp\GR6250-2019\hw6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4608A07A-8C6C-443A-86EF-D4C1E7FA7919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC61B29-DDC0-4FFB-AE07-F04034F24550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{D3B39B31-0FCC-485C-968B-EB7A4BAB9E1D}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>General Option Pricing</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>x_</t>
   </si>
 </sst>
 </file>
@@ -430,14 +433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0254B9-6FD0-4A8A-AD90-E09EBAA5AE26}">
-  <dimension ref="B2:L106"/>
+  <dimension ref="B2:L108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
@@ -452,7 +456,7 @@
         <v>6</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.45">
@@ -460,7 +464,18 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>1</v>
+      </c>
+      <c r="D4" cm="1">
+        <f t="array" ref="D4:D6">_xll.XLL.CUMULANT.NORMALIZE(C6)</f>
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <f>(F3-D4)/D5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.45">
@@ -468,7 +483,10 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="D5">
+        <v>0.31622776601683794</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -483,15 +501,22 @@
       </c>
       <c r="C6" cm="1">
         <f t="array" ref="C6">_xll.XLL.CUMULANT.POISSON(C5,C4)</f>
-        <v>32431824</v>
+        <v>29179580</v>
+      </c>
+      <c r="D6">
+        <v>28651638</v>
       </c>
       <c r="E6" cm="1">
-        <f t="array" ref="E6">_xll.XLL.BELL.REDUCED(C6)</f>
-        <v>32034718</v>
+        <f t="array" ref="E6">_xll.XLL.BELL.REDUCED(D6,{1,0,0})</f>
+        <v>30145922</v>
       </c>
       <c r="F6" cm="1">
         <f t="array" ref="F6">_xll.XLL.HERMITE(F3)</f>
-        <v>31428938</v>
+        <v>-1365472</v>
+      </c>
+      <c r="G6" cm="1">
+        <f t="array" ref="G6">_xll.XLL.SEQUENCE.MUL(E6,F6)</f>
+        <v>29657044</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.45">
@@ -510,1655 +535,1707 @@
         <f t="array" ref="F7:F106">_xll.XLL.SEQUENCE.TAKE(B7,F6)</f>
         <v>1</v>
       </c>
-      <c r="G7">
-        <f>E7*F7</f>
+      <c r="G7" cm="1">
+        <f t="array" ref="G7:G106">_xll.XLL.SEQUENCE.TAKE(B7,G6)</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C8">
-        <v>1.0000000000000002E-2</v>
+        <v>0.1</v>
       </c>
       <c r="E8">
-        <v>1.0000000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="F8">
+        <v>0.1</v>
+      </c>
+      <c r="G8">
         <v>0</v>
-      </c>
-      <c r="G8">
-        <f>E8*F8+G7</f>
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C9">
-        <v>1.0000000000000002E-3</v>
+        <v>0.1</v>
+      </c>
+      <c r="D9" cm="1">
+        <f t="array" ref="D9:D108">_xll.XLL.SEQUENCE.TAKE(B7,D6)</f>
+        <v>3.1622776601683791</v>
       </c>
       <c r="E9">
-        <v>5.5000000000000014E-4</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>-1</v>
+        <v>-0.99</v>
       </c>
       <c r="G9">
-        <f>E9*F9+G8</f>
-        <v>0.99944999999999995</v>
-      </c>
-      <c r="K9">
-        <v>-0.1</v>
-      </c>
-      <c r="L9" cm="1">
-        <f t="array" ref="L9">_xll.XLL.OPTION.PDF(K8, $C$6)</f>
-        <v>-9.9227215334176574E+33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C10">
-        <v>1.0000000000000003E-4</v>
+        <v>0.1</v>
+      </c>
+      <c r="D10">
+        <v>9.9999999999999982</v>
       </c>
       <c r="E10">
-        <v>2.183333333333334E-5</v>
+        <v>16.666666666666661</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>-0.29900000000000004</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G9:G72" si="0">E10*F10+G9</f>
-        <v>0.99944999999999995</v>
+        <v>-4.9833333333333325</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" cm="1">
-        <f t="array" ref="L10">_xll.XLL.OPTION.PDF(K9, $C$6)</f>
-        <v>1.4405908515909151E+34</v>
+        <f t="array" ref="L10">_xll.XLL.OPTION.PDF(F3, $C$6)</f>
+        <v>-77.5003130223743</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C11">
-        <v>1.0000000000000004E-5</v>
+        <v>0.1</v>
+      </c>
+      <c r="D11">
+        <v>31.622776601683785</v>
       </c>
       <c r="E11">
-        <v>7.3375000000000039E-7</v>
+        <v>54.842823584034882</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>2.9400999999999997</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
-        <v>0.99945220124999989</v>
-      </c>
-      <c r="K11">
-        <v>0.1</v>
-      </c>
-      <c r="L11" cm="1">
-        <f t="array" ref="L11">_xll.XLL.OPTION.PDF(K10, $C$6)</f>
-        <v>-9.9227215334176574E+33</v>
+        <v>161.24338561942093</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C12">
-        <v>1.0000000000000004E-6</v>
+        <v>0.1</v>
+      </c>
+      <c r="D12">
+        <v>99.999999999999972</v>
       </c>
       <c r="E12">
-        <v>2.3000833333333344E-8</v>
+        <v>223.428235840349</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1.4900100000000003</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
-        <v>0.99945220124999989</v>
-      </c>
-      <c r="K12">
-        <v>0.2</v>
-      </c>
-      <c r="L12" cm="1">
-        <f t="array" ref="L12">_xll.XLL.OPTION.PDF(K11, $C$6)</f>
-        <v>0.58179082558542139</v>
+        <v>332.91030568447849</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C13">
-        <v>1.0000000000000005E-7</v>
+        <v>0.1</v>
+      </c>
+      <c r="D13">
+        <v>316.22776601683779</v>
       </c>
       <c r="E13">
-        <v>7.03681944444445E-10</v>
+        <v>804.70839399584145</v>
       </c>
       <c r="F13">
-        <v>-15</v>
+        <v>-14.551498999999998</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0.99945219069477076</v>
-      </c>
-      <c r="K13">
-        <v>0.3</v>
-      </c>
-      <c r="L13" cm="1">
-        <f t="array" ref="L13">_xll.XLL.OPTION.PDF(K12, $C$6)</f>
-        <v>3.6213632350708721E+34</v>
+        <v>-11709.713390522091</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C14">
-        <v>1.0000000000000005E-8</v>
+        <v>0.1</v>
+      </c>
+      <c r="D14">
+        <v>999.99999999999943</v>
       </c>
       <c r="E14">
-        <v>2.1178990079365091E-11</v>
+        <v>2678.1350939563722</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>-10.395209900000003</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
-        <v>0.99945219069477076</v>
-      </c>
-      <c r="K14">
-        <v>0.4</v>
-      </c>
-      <c r="L14" cm="1">
-        <f t="array" ref="L14">_xll.XLL.OPTION.PDF(K13, $C$6)</f>
-        <v>-2.2250163299225398E+34</v>
+        <v>-27839.77644223272</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C15">
-        <v>1.0000000000000005E-9</v>
+        <v>0.1</v>
+      </c>
+      <c r="D15">
+        <v>3162.2776601683772</v>
       </c>
       <c r="E15">
-        <v>6.2422341517857187E-13</v>
+        <v>8373.8832383289791</v>
       </c>
       <c r="F15">
-        <v>105</v>
+        <v>100.82097200999999</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
-        <v>0.99945219076031422</v>
-      </c>
-      <c r="K15">
-        <v>0.5</v>
-      </c>
-      <c r="L15" cm="1">
-        <f t="array" ref="L15">_xll.XLL.OPTION.PDF(K14, $C$6)</f>
-        <v>6.2724646659124135E+33</v>
+        <v>844263.0475865741</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C16">
-        <v>1.0000000000000006E-10</v>
+        <v>0.1</v>
+      </c>
+      <c r="D16">
+        <v>9999.9999999999927</v>
       </c>
       <c r="E16">
-        <v>1.7978953265542349E-14</v>
+        <v>24796.313876427808</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>93.243776401000019</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
-        <v>0.99945219076031422</v>
-      </c>
-      <c r="K16">
-        <v>0.6</v>
-      </c>
-      <c r="L16" cm="1">
-        <f t="array" ref="L16">_xll.XLL.OPTION.PDF(K15, $C$6)</f>
-        <v>-8.8824803052845773E+32</v>
-      </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.45">
+        <v>2312101.9466626486</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C17">
-        <v>1.0000000000000006E-11</v>
+        <v>0.1</v>
+      </c>
+      <c r="D17">
+        <v>31622.776601683767</v>
       </c>
       <c r="E17">
-        <v>5.0703187128251816E-16</v>
+        <v>70007.428673019051</v>
       </c>
       <c r="F17">
-        <v>-945</v>
+        <v>-898.06437044989991</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983505</v>
-      </c>
-      <c r="K17">
-        <v>0.7</v>
-      </c>
-      <c r="L17" cm="1">
-        <f t="array" ref="L17">_xll.XLL.OPTION.PDF(K16, $C$6)</f>
-        <v>6.7889879008481343E+31</v>
-      </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.45">
+        <v>-62871177.358051129</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C18">
-        <v>1.0000000000000006E-12</v>
+        <v>0.1</v>
+      </c>
+      <c r="D18">
+        <v>99999.999999999927</v>
       </c>
       <c r="E18">
-        <v>1.404403801419704E-17</v>
+        <v>189484.61612898347</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>-1022.2442010549901</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983505</v>
-      </c>
-      <c r="K18">
-        <v>0.8</v>
-      </c>
-      <c r="L18" cm="1">
-        <f t="array" ref="L18">_xll.XLL.OPTION.PDF(K17, $C$6)</f>
-        <v>-3.2536720420139308E+30</v>
-      </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.45">
+        <v>-193699550.02698418</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C19">
-        <v>1.0000000000000007E-13</v>
+        <v>0.1</v>
+      </c>
+      <c r="D19">
+        <v>316227.76601683762</v>
       </c>
       <c r="E19">
-        <v>3.8293839585538177E-19</v>
+        <v>493843.09249147674</v>
       </c>
       <c r="F19">
-        <v>10395</v>
+        <v>9776.4836548434014</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K19">
-        <v>0.9</v>
-      </c>
-      <c r="L19" cm="1">
-        <f t="array" ref="L19">_xll.XLL.OPTION.PDF(K18, $C$6)</f>
-        <v>1.2821205836774032E+29</v>
-      </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.45">
+        <v>4828048921.8002405</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C20">
-        <v>1.0000000000000008E-14</v>
+        <v>0.1</v>
+      </c>
+      <c r="D20">
+        <v>999999.99999999895</v>
       </c>
       <c r="E20">
-        <v>1.0292646268001688E-20</v>
+        <v>1243840.6408390945</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>13244.57877814422</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20" cm="1">
-        <f t="array" ref="L20">_xll.XLL.OPTION.PDF(K19, $C$6)</f>
-        <v>-4.4072273463778521E+27</v>
-      </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.45">
+        <v>16474145355.050777</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C21">
-        <v>1.0000000000000009E-15</v>
+        <v>0.1</v>
+      </c>
+      <c r="D21">
+        <v>3162277.6601683758</v>
       </c>
       <c r="E21">
-        <v>2.729450706725069E-22</v>
+        <v>3036838.9492958165</v>
       </c>
       <c r="F21">
-        <v>-135135</v>
+        <v>-125769.8296351498</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K21">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="L21" cm="1">
-        <f t="array" ref="L21">_xll.XLL.OPTION.PDF(K20, $C$6)</f>
-        <v>9.8699901467224828E+25</v>
-      </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.45">
+        <v>-381942717282.32214</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C22">
-        <v>1.000000000000001E-16</v>
+        <v>0.1</v>
+      </c>
+      <c r="D22">
+        <v>9999999.9999999888</v>
       </c>
       <c r="E22">
-        <v>7.1471136263464007E-24</v>
+        <v>7205779.0583372582</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>-198001.08585753405</v>
       </c>
       <c r="G22">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K22">
-        <v>1.2</v>
-      </c>
-      <c r="L22" cm="1">
-        <f t="array" ref="L22">_xll.XLL.OPTION.PDF(K21, $C$6)</f>
-        <v>-1.0612864437598611E+24</v>
-      </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.45">
+        <v>-1426752078000.2563</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C23">
-        <v>1.000000000000001E-17</v>
+        <v>0.1</v>
+      </c>
+      <c r="D23">
+        <v>31622776.601683758</v>
       </c>
       <c r="E23">
-        <v>1.8494963968937922E-25</v>
+        <v>16653457.025567412</v>
       </c>
       <c r="F23">
-        <v>2027025</v>
+        <v>1866747.3359414935</v>
       </c>
       <c r="G23">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K23">
-        <v>1.3</v>
-      </c>
-      <c r="L23" cm="1">
-        <f t="array" ref="L23">_xll.XLL.OPTION.PDF(K22, $C$6)</f>
-        <v>3.0390785229099919E+21</v>
-      </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.45">
+        <v>31087796536694.117</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C24">
-        <v>1.000000000000001E-18</v>
+        <v>0.1</v>
+      </c>
+      <c r="D24">
+        <v>99999999.999999866</v>
       </c>
       <c r="E24">
-        <v>4.7335114310051508E-27</v>
+        <v>37560048.238612562</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>3354692.1073146942</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K24">
-        <v>1.4</v>
-      </c>
-      <c r="L24" cm="1">
-        <f t="array" ref="L24">_xll.XLL.OPTION.PDF(K23, $C$6)</f>
-        <v>1.2970143532927969E+19</v>
-      </c>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.45">
+        <v>126002397376432.75</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C25">
-        <v>1.0000000000000011E-19</v>
+        <v>0.1</v>
+      </c>
+      <c r="D25">
+        <v>316227766.01683748</v>
       </c>
       <c r="E25">
-        <v>1.1990010909289731E-28</v>
+        <v>82808591.088176101</v>
       </c>
       <c r="F25">
-        <v>-34459425</v>
+        <v>-31399235.500273921</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K25">
-        <v>1.5</v>
-      </c>
-      <c r="L25" cm="1">
-        <f t="array" ref="L25">_xll.XLL.OPTION.PDF(K24, $C$6)</f>
-        <v>-2.6792446013986952E+16</v>
-      </c>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.45">
+        <v>-2600126453023525.5</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C26">
-        <v>1.0000000000000011E-20</v>
+        <v>0.1</v>
+      </c>
+      <c r="D26">
+        <v>999999999.99999845</v>
       </c>
       <c r="E26">
-        <v>3.007597016503495E-30</v>
+        <v>178728858.77149701</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>-63524381.481691889</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K26">
-        <v>1.6</v>
-      </c>
-      <c r="L26" cm="1">
-        <f t="array" ref="L26">_xll.XLL.OPTION.PDF(K25, $C$6)</f>
-        <v>-47700080195454.617</v>
-      </c>
-    </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.45">
+        <v>-1.135364020638801E+16</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C27">
-        <v>1.0000000000000012E-21</v>
+        <v>0.1</v>
+      </c>
+      <c r="D27">
+        <v>3162277660.1683741</v>
       </c>
       <c r="E27">
-        <v>7.4749775960183687E-32</v>
+        <v>378141199.27136135</v>
       </c>
       <c r="F27">
-        <v>654729075</v>
+        <v>590233036.35703528</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K27">
-        <v>1.7</v>
-      </c>
-      <c r="L27" cm="1">
-        <f t="array" ref="L27">_xll.XLL.OPTION.PDF(K26, $C$6)</f>
-        <v>-26583121246.947403</v>
-      </c>
-    </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.45">
+        <v>2.2319142821762634E+17</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C28">
-        <v>1.0000000000000012E-22</v>
+        <v>0.1</v>
+      </c>
+      <c r="D28">
+        <v>9999999999.9999828</v>
       </c>
       <c r="E28">
-        <v>1.8415967667773798E-33</v>
+        <v>785167127.3641845</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1329510933.2695413</v>
       </c>
       <c r="G28">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K28">
-        <v>1.8</v>
-      </c>
-      <c r="L28" cm="1">
-        <f t="array" ref="L28">_xll.XLL.OPTION.PDF(K27, $C$6)</f>
-        <v>-12721533.938917112</v>
-      </c>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.45">
+        <v>1.0438882802745217E+18</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C29">
-        <v>1.0000000000000013E-23</v>
+        <v>0.1</v>
+      </c>
+      <c r="D29">
+        <v>31622776601.683735</v>
       </c>
       <c r="E29">
-        <v>4.4994628546167933E-35</v>
+        <v>1601679639.4255438</v>
       </c>
       <c r="F29">
-        <v>-13749310575</v>
+        <v>-12261942670.170788</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K29">
-        <v>1.9</v>
-      </c>
-      <c r="L29" cm="1">
-        <f t="array" ref="L29">_xll.XLL.OPTION.PDF(K28, $C$6)</f>
-        <v>-4999.3426286965796</v>
-      </c>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.45">
+        <v>-1.9639703914615837E+19</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C30">
-        <v>1.0000000000000014E-24</v>
+        <v>0.1</v>
+      </c>
+      <c r="D30">
+        <v>99999999999.999802</v>
       </c>
       <c r="E30">
-        <v>1.0906363008193103E-36</v>
+        <v>3212969098.2472124</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>-30475434798.946987</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K30">
-        <v>2</v>
-      </c>
-      <c r="L30" cm="1">
-        <f t="array" ref="L30">_xll.XLL.OPTION.PDF(K29, $C$6)</f>
-        <v>-6.8467367089198025E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.45">
+        <v>-9.7916630264664424E+19</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C31">
-        <v>1.0000000000000014E-25</v>
+        <v>0.1</v>
+      </c>
+      <c r="D31">
+        <v>316227766016.83728</v>
       </c>
       <c r="E31">
-        <v>2.6236719120914556E-38</v>
+        <v>6343487121.283843</v>
       </c>
       <c r="F31">
-        <v>316234143225</v>
+        <v>278977137934.03339</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
-      </c>
-      <c r="K31">
-        <v>2.1</v>
-      </c>
-      <c r="L31" cm="1">
-        <f t="array" ref="L31">_xll.XLL.OPTION.PDF(K30, $C$6)</f>
-        <v>6.1662350131166051E-5</v>
-      </c>
-    </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.45">
+        <v>1.7696878816171671E+21</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C32">
-        <v>1.0000000000000015E-26</v>
+        <v>0.1</v>
+      </c>
+      <c r="D32">
+        <v>999999999999.9978</v>
       </c>
       <c r="E32">
-        <v>6.2660412722298508E-40</v>
+        <v>12336156583.07688</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>759308148968.13098</v>
       </c>
       <c r="G32">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>9.3669442204771287E+21</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C33">
-        <v>1.0000000000000015E-27</v>
+        <v>0.1</v>
+      </c>
+      <c r="D33">
+        <v>3162277660168.3721</v>
       </c>
       <c r="E33">
-        <v>1.4861520592258813E-41</v>
+        <v>23646794500.094364</v>
       </c>
       <c r="F33">
-        <v>-7905853580625</v>
+        <v>-6898497633454.0215</v>
       </c>
       <c r="G33">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-1.6312735589767454E+23</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C34">
-        <v>1.0000000000000015E-28</v>
+        <v>0.1</v>
+      </c>
+      <c r="D34">
+        <v>9999999999999.9766</v>
       </c>
       <c r="E34">
-        <v>3.5013977794104231E-43</v>
+        <v>44708462874.090202</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>-20431861636516.809</v>
       </c>
       <c r="G34">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-9.1347712742475957E+23</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C35">
-        <v>1.0000000000000016E-29</v>
+        <v>0.1</v>
+      </c>
+      <c r="D35">
+        <v>31622776601683.715</v>
       </c>
       <c r="E35">
-        <v>8.1967344500130457E-45</v>
+        <v>83424554661.785324</v>
       </c>
       <c r="F35">
-        <v>213458046676875</v>
+        <v>184216249939606.91</v>
       </c>
       <c r="G35">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>1.5368158612675845E+25</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C36">
-        <v>1.0000000000000017E-30</v>
+        <v>0.1</v>
+      </c>
+      <c r="D36">
+        <v>99999999999999.734</v>
       </c>
       <c r="E36">
-        <v>1.9070694499327684E-46</v>
+        <v>153718497770.65823</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>590513750816431.38</v>
       </c>
       <c r="G36">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>9.077288668841863E+25</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C37">
-        <v>1.0000000000000016E-31</v>
+        <v>0.1</v>
+      </c>
+      <c r="D37">
+        <v>316227766016837.13</v>
       </c>
       <c r="E37">
-        <v>4.4107880424278018E-48</v>
+        <v>279839980237.88007</v>
       </c>
       <c r="F37">
-        <v>-6190283353629375</v>
+        <v>-5283219873166957</v>
       </c>
       <c r="G37">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-1.4784561448994165E+27</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C38">
-        <v>1.0000000000000017E-32</v>
+        <v>0.1</v>
+      </c>
+      <c r="D38">
+        <v>999999999999997.5</v>
       </c>
       <c r="E38">
-        <v>1.0143344190498391E-49</v>
+        <v>503560831538.18988</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>-1.8243734511809636E+16</v>
       </c>
       <c r="G38">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-9.1868301211288328E+27</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C39">
-        <v>1.0000000000000018E-33</v>
+        <v>0.1</v>
+      </c>
+      <c r="D39">
+        <v>3162277660168371</v>
       </c>
       <c r="E39">
-        <v>2.3197797543799589E-51</v>
+        <v>896076957629.67297</v>
       </c>
       <c r="F39">
-        <v>1.9189878396251062E+17</v>
+        <v>1.6195544261699472E+17</v>
       </c>
       <c r="G39">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>1.4512454029180372E+29</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C40">
-        <v>1.0000000000000019E-34</v>
+        <v>0.1</v>
+      </c>
+      <c r="D40">
+        <v>9999999999999972</v>
       </c>
       <c r="E40">
-        <v>5.2770706120482573E-53</v>
+        <v>1577500165472.9888</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>5.9999504863960781E+17</v>
       </c>
       <c r="G40">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>9.4649228851195521E+29</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C41">
-        <v>1.0000000000000019E-35</v>
+        <v>0.1</v>
+      </c>
+      <c r="D41">
+        <v>3.1622776601683704E+16</v>
       </c>
       <c r="E41">
-        <v>1.1942484145293182E-54</v>
+        <v>2748476114928.8667</v>
       </c>
       <c r="F41">
-        <v>-6.3326598707628503E+18</v>
+        <v>-5.2845301014968648E+18</v>
       </c>
       <c r="G41">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-1.4524404762586752E+31</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C42">
-        <v>1.0000000000000019E-36</v>
+        <v>0.1</v>
+      </c>
+      <c r="D42">
+        <v>9.9999999999999712E+16</v>
       </c>
       <c r="E42">
-        <v>2.6891972481597652E-56</v>
+        <v>4740999934010.7979</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>-2.0928284663896351E+19</v>
       </c>
       <c r="G42">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-9.9220996210491799E+31</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C43">
-        <v>1.0000000000000019E-37</v>
+        <v>0.1</v>
+      </c>
+      <c r="D43">
+        <v>3.1622776601683699E+17</v>
       </c>
       <c r="E43">
-        <v>6.0261978013210971E-58</v>
+        <v>8099357568166.1182</v>
       </c>
       <c r="F43">
-        <v>2.2164309547669976E+20</v>
+        <v>1.8286572508600061E+20</v>
       </c>
       <c r="G43">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>1.4810948944334837E+33</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C44">
-        <v>1.0000000000000021E-38</v>
+        <v>0.1</v>
+      </c>
+      <c r="D44">
+        <v>9.9999999999999693E+17</v>
       </c>
       <c r="E44">
-        <v>1.3440630027286051E-59</v>
+        <v>13707938325515.389</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>7.7170482040886867E+20</v>
       </c>
       <c r="G44">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>1.0578482083667701E+34</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C45">
-        <v>1.0000000000000021E-39</v>
+        <v>0.1</v>
+      </c>
+      <c r="D45">
+        <v>3.1622776601683692E+18</v>
       </c>
       <c r="E45">
-        <v>2.9840818198484656E-61</v>
+        <v>22991368176201.898</v>
       </c>
       <c r="F45">
-        <v>-8.2007945326378908E+21</v>
+        <v>-6.6888613461411349E+21</v>
       </c>
       <c r="G45">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-1.5378607388869629E+35</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C46">
-        <v>1.0000000000000022E-40</v>
+        <v>0.1</v>
+      </c>
+      <c r="D46">
+        <v>9.9999999999999672E+18</v>
       </c>
       <c r="E46">
-        <v>6.5958815283624017E-63</v>
+        <v>38225333861243.734</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>-2.9993669310151123E+22</v>
       </c>
       <c r="G46">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-1.1465180231042667E+36</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C47">
-        <v>1.0000000000000022E-41</v>
+        <v>0.1</v>
+      </c>
+      <c r="D47">
+        <v>3.1622776601683685E+19</v>
       </c>
       <c r="E47">
-        <v>1.4516409795915453E-64</v>
+        <v>63015499904310.922</v>
       </c>
       <c r="F47">
-        <v>3.1983098677287775E+23</v>
+        <v>2.5786622556848913E+23</v>
       </c>
       <c r="G47">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>1.6249569112636145E+37</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C48">
-        <v>1.0000000000000023E-42</v>
+        <v>0.1</v>
+      </c>
+      <c r="D48">
+        <v>9.999999999999964E+19</v>
       </c>
       <c r="E48">
-        <v>3.1814153394562092E-66</v>
+        <v>103029745116261.64</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>1.2255333949628937E+24</v>
       </c>
       <c r="G48">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>1.2626639331449374E+38</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C49">
-        <v>1.0000000000000023E-43</v>
+        <v>0.1</v>
+      </c>
+      <c r="D49">
+        <v>3.1622776601683683E+20</v>
       </c>
       <c r="E49">
-        <v>6.9439136516740888E-68</v>
+        <v>167109327020735.06</v>
       </c>
       <c r="F49">
-        <v>-1.3113070457687988E+25</v>
+        <v>-1.0449961908811764E+25</v>
       </c>
       <c r="G49">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-1.7462861019738498E+39</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C50">
-        <v>1.0000000000000023E-44</v>
+        <v>0.1</v>
+      </c>
+      <c r="D50">
+        <v>9.9999999999999646E+20</v>
       </c>
       <c r="E50">
-        <v>1.5095820477863916E-69</v>
+        <v>268942771260570.13</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>-5.2517398779322711E+25</v>
       </c>
       <c r="G50">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-1.4124174767107533E+40</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C51">
-        <v>1.0000000000000023E-45</v>
+        <v>0.1</v>
+      </c>
+      <c r="D51">
+        <v>3.1622776601683679E+21</v>
       </c>
       <c r="E51">
-        <v>3.2690466115548737E-71</v>
+        <v>429569546802828.94</v>
       </c>
       <c r="F51">
-        <v>5.6386202968058344E+26</v>
+        <v>4.4409662220097358E+26</v>
       </c>
       <c r="G51">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>1.9077038473553938E+41</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C52">
-        <v>1.0000000000000024E-46</v>
+        <v>0.1</v>
+      </c>
+      <c r="D52">
+        <v>9.9999999999999623E+21</v>
       </c>
       <c r="E52">
-        <v>7.0524330393953951E-73</v>
+        <v>681098921469461.38</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>2.3551752085102968E+27</v>
       </c>
       <c r="G52">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>1.604107294387977E+42</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C53">
-        <v>1.0000000000000024E-47</v>
+        <v>0.1</v>
+      </c>
+      <c r="D53">
+        <v>3.1622776601683671E+22</v>
       </c>
       <c r="E53">
-        <v>1.5158279092661522E-74</v>
+        <v>1072196447850081.4</v>
       </c>
       <c r="F53">
-        <v>-2.5373791335626256E+28</v>
+        <v>-1.9748830478192784E+28</v>
       </c>
       <c r="G53">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-2.1174625887911728E+43</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C54">
-        <v>1.0000000000000024E-48</v>
+        <v>0.1</v>
+      </c>
+      <c r="D54">
+        <v>9.9999999999999589E+22</v>
       </c>
       <c r="E54">
-        <v>3.2463230397851563E-76</v>
+        <v>1676124831206619</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>-1.1031294263929292E+29</v>
       </c>
       <c r="G54">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-1.848982623611903E+44</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C55">
-        <v>1.0000000000000024E-49</v>
+        <v>0.1</v>
+      </c>
+      <c r="D55">
+        <v>3.1622776601683666E+23</v>
       </c>
       <c r="E55">
-        <v>6.9278849122206339E-78</v>
+        <v>2602452451415247.5</v>
       </c>
       <c r="F55">
-        <v>1.192568192774434E+30</v>
+        <v>9.1716373821113162E+29</v>
       </c>
       <c r="G55">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>2.3868750188567317E+45</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C56">
-        <v>1.0000000000000025E-50</v>
+        <v>0.1</v>
+      </c>
+      <c r="D56">
+        <v>9.9999999999999582E+23</v>
       </c>
       <c r="E56">
-        <v>1.4733683338708848E-79</v>
+        <v>4013995002609410</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>5.3867376205071732E+30</v>
       </c>
       <c r="G56">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>2.1622337889083899E+46</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C57">
-        <v>1.0000000000000025E-51</v>
+        <v>0.1</v>
+      </c>
+      <c r="D57">
+        <v>3.1622776601683656E+24</v>
       </c>
       <c r="E57">
-        <v>3.1228917151626295E-81</v>
+        <v>6151178107493286</v>
       </c>
       <c r="F57">
-        <v>-5.8435841445947271E+31</v>
+        <v>-4.4402349410294729E+31</v>
       </c>
       <c r="G57">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-2.7312675961387234E+47</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C58">
-        <v>1.0000000000000026E-52</v>
+        <v>0.1</v>
+      </c>
+      <c r="D58">
+        <v>9.9999999999999558E+24</v>
       </c>
       <c r="E58">
-        <v>6.5973461686110959E-83</v>
+        <v>9366860270486912</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>-2.7377711596638814E+32</v>
       </c>
       <c r="G58">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-2.5644319905140492E+48</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C59">
-        <v>1.0000000000000027E-53</v>
+        <v>0.1</v>
+      </c>
+      <c r="D59">
+        <v>3.1622776601683653E+25</v>
       </c>
       <c r="E59">
-        <v>1.3892452350147856E-84</v>
+        <v>1.4175813620431232E+16</v>
       </c>
       <c r="F59">
-        <v>2.9802279137433107E+33</v>
+        <v>2.2371421083283923E+33</v>
       </c>
       <c r="G59">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>3.1713309570081865E+49</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C60">
-        <v>1.0000000000000028E-54</v>
+        <v>0.1</v>
+      </c>
+      <c r="D60">
+        <v>9.9999999999999524E+25</v>
       </c>
       <c r="E60">
-        <v>2.9161857984617647E-86</v>
+        <v>2.1324625811508404E+16</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>1.4460124241085023E+34</v>
       </c>
       <c r="G60">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>3.0835673862906005E+50</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C61">
-        <v>1.0000000000000029E-55</v>
+        <v>0.1</v>
+      </c>
+      <c r="D61">
+        <v>3.1622776601683645E+26</v>
       </c>
       <c r="E61">
-        <v>6.1024789848149774E-88</v>
+        <v>3.1889891760771748E+16</v>
       </c>
       <c r="F61">
-        <v>-1.5795207942839547E+35</v>
+        <v>-1.1712251931729629E+35</v>
       </c>
       <c r="G61">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-3.7350244637774771E+51</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C62">
-        <v>1.000000000000003E-56</v>
+        <v>0.1</v>
+      </c>
+      <c r="D62">
+        <v>9.999999999999952E+26</v>
       </c>
       <c r="E62">
-        <v>1.2731493174696376E-89</v>
+        <v>4.7415378546113E+16</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>-7.9255896095032091E+35</v>
       </c>
       <c r="G62">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-3.7579483153573455E+52</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C63">
-        <v>1.0000000000000031E-57</v>
+        <v>0.1</v>
+      </c>
+      <c r="D63">
+        <v>3.1622776601683634E+27</v>
       </c>
       <c r="E63">
-        <v>2.6482589073729561E-91</v>
+        <v>7.0102589029275824E+16</v>
       </c>
       <c r="F63">
-        <v>8.6873643685617512E+36</v>
+        <v>6.3624826663562634E+36</v>
       </c>
       <c r="G63">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>4.4602650756546416E+53</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C64">
-        <v>1.0000000000000032E-58</v>
+        <v>0.1</v>
+      </c>
+      <c r="D64">
+        <v>9.9999999999999512E+27</v>
       </c>
       <c r="E64">
-        <v>5.4925590612842715E-93</v>
+        <v>1.030740983169431E+17</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>4.5019550079853601E+37</v>
       </c>
       <c r="G64">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>4.640349531115374E+54</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C65">
-        <v>1.0000000000000033E-59</v>
+        <v>0.1</v>
+      </c>
+      <c r="D65">
+        <v>3.1622776601683636E+28</v>
       </c>
       <c r="E65">
-        <v>1.135916624672331E-94</v>
+        <v>1.5073554592695907E+17</v>
       </c>
       <c r="F65">
-        <v>-4.9517976900801979E+38</v>
+        <v>-3.5815955697432162E+38</v>
       </c>
       <c r="G65">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-5.3987376349482176E+55</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C66">
-        <v>1.0000000000000034E-60</v>
+        <v>0.1</v>
+      </c>
+      <c r="D66">
+        <v>9.9999999999999499E+28</v>
       </c>
       <c r="E66">
-        <v>2.3426044940388697E-96</v>
+        <v>2.1927068233617334E+17</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>-2.646949860328941E+39</v>
       </c>
       <c r="G66">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-5.8039850198396561E+56</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C67">
-        <v>1.0000000000000035E-61</v>
+        <v>0.1</v>
+      </c>
+      <c r="D67">
+        <v>3.1622776601683636E+29</v>
       </c>
       <c r="E67">
-        <v>4.8178673307930407E-98</v>
+        <v>3.1731495253310502E+17</v>
       </c>
       <c r="F67">
-        <v>2.9215606371473166E+40</v>
+        <v>2.0866718875452082E+40</v>
       </c>
       <c r="G67">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>6.6213219094857246E+57</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C68">
-        <v>1.0000000000000035E-62</v>
+        <v>0.1</v>
+      </c>
+      <c r="D68">
+        <v>9.9999999999999481E+29</v>
       </c>
       <c r="E68">
-        <v>9.8817946493361583E-100</v>
+        <v>4.5686745191394464E+17</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>1.6090366350728168E+41</v>
       </c>
       <c r="G68">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>7.3511646750190543E+58</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C69">
-        <v>1.0000000000000036E-63</v>
+        <v>0.1</v>
+      </c>
+      <c r="D69">
+        <v>3.1622776601683627E+30</v>
       </c>
       <c r="E69">
-        <v>2.0214498588519309E-101</v>
+        <v>6.5451958143841587E+17</v>
       </c>
       <c r="F69">
-        <v>-1.7821519886598631E+42</v>
+        <v>-1.2567794850518488E+42</v>
       </c>
       <c r="G69">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-8.2258678251652392E+59</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C70">
-        <v>1.0000000000000037E-64</v>
+        <v>0.1</v>
+      </c>
+      <c r="D70">
+        <v>9.9999999999999467E+30</v>
       </c>
       <c r="E70">
-        <v>4.124360491522491E-103</v>
+        <v>9.3310243405631642E+17</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>-1.0101705085956649E+43</v>
       </c>
       <c r="G70">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>-9.4259256038252208E+60</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C71">
-        <v>1.0000000000000037E-65</v>
+        <v>0.1</v>
+      </c>
+      <c r="D71">
+        <v>3.1622776601683627E+31</v>
       </c>
       <c r="E71">
-        <v>8.3933711175076512E-105</v>
+        <v>1.3238851831235328E+18</v>
       </c>
       <c r="F71">
-        <v>1.1227557528557138E+44</v>
+        <v>7.8166937049670814E+43</v>
       </c>
       <c r="G71">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>1.034840497702091E+62</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C72">
-        <v>1.0000000000000038E-66</v>
+        <v>0.1</v>
+      </c>
+      <c r="D72">
+        <v>9.9999999999999447E+31</v>
       </c>
       <c r="E72">
-        <v>1.7038110442403704E-106</v>
+        <v>1.8694951286661445E+18</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>6.5432581920619258E+44</v>
       </c>
       <c r="G72">
-        <f t="shared" si="0"/>
-        <v>0.99945219075983904</v>
+        <v>1.2232589315664615E+63</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C73">
-        <v>1.0000000000000039E-67</v>
+        <v>0.1</v>
+      </c>
+      <c r="D73">
+        <v>3.1622776601683615E+32</v>
       </c>
       <c r="E73">
-        <v>3.4500870399686544E-108</v>
+        <v>2.6277785487179576E+18</v>
       </c>
       <c r="F73">
-        <v>-7.2979123935621403E+45</v>
+        <v>-5.0154183263079837E+45</v>
       </c>
       <c r="G73">
-        <f t="shared" ref="G73:G106" si="1">E73*F73+G72</f>
-        <v>0.99945219075983904</v>
+        <v>-1.3179408690719041E+64</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C74">
-        <v>1.000000000000004E-68</v>
+        <v>0.1</v>
+      </c>
+      <c r="D74">
+        <v>9.9999999999999447E+32</v>
       </c>
       <c r="E74">
-        <v>6.9691552732590846E-110</v>
+        <v>3.6768824690998892E+18</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>-4.3687045900239509E+46</v>
       </c>
       <c r="G74">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-1.6063213319735283E+65</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C75">
-        <v>1.0000000000000041E-69</v>
+        <v>0.1</v>
+      </c>
+      <c r="D75">
+        <v>3.1622776601683613E+33</v>
       </c>
       <c r="E75">
-        <v>1.4043940813757556E-111</v>
+        <v>5.1219137529996503E+18</v>
       </c>
       <c r="F75">
-        <v>4.8896013036866339E+47</v>
+        <v>3.3166432327261096E+47</v>
       </c>
       <c r="G75">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>1.698756058749308E+66</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C76">
-        <v>1.0000000000000042E-70</v>
+        <v>0.1</v>
+      </c>
+      <c r="D76">
+        <v>9.9999999999999418E+33</v>
       </c>
       <c r="E76">
-        <v>2.8234062271958951E-113</v>
+        <v>7.1036269252511805E+18</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>3.0038855535435478E+48</v>
       </c>
       <c r="G76">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>2.1338482298524992E+67</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C77">
-        <v>1.0000000000000041E-71</v>
+        <v>0.1</v>
+      </c>
+      <c r="D77">
+        <v>3.1622776601683613E+34</v>
       </c>
       <c r="E77">
-        <v>5.6630387978248269E-115</v>
+        <v>9.8097099323040113E+18</v>
       </c>
       <c r="F77">
-        <v>-3.3738248995437775E+49</v>
+        <v>-2.2584449750455802E+49</v>
       </c>
       <c r="G77">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-2.2154690103266712E+68</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C78">
-        <v>1.0000000000000042E-72</v>
+        <v>0.1</v>
+      </c>
+      <c r="D78">
+        <v>9.9999999999999407E+34</v>
       </c>
       <c r="E78">
-        <v>1.1332697016242816E-116</v>
+        <v>1.3489382383018002E+19</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>-2.1253043372309395E+50</v>
       </c>
       <c r="G78">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-2.8669042885194786E+69</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C79">
-        <v>1.0000000000000042E-73</v>
+        <v>0.1</v>
+      </c>
+      <c r="D79">
+        <v>3.1622776601683603E+35</v>
       </c>
       <c r="E79">
-        <v>2.2627673867155985E-118</v>
+        <v>1.8472199345134035E+19</v>
       </c>
       <c r="F79">
-        <v>2.395415678676082E+51</v>
+        <v>1.5822428889100523E+51</v>
       </c>
       <c r="G79">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>2.9227506056367251E+70</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C80">
-        <v>1.0000000000000043E-74</v>
+        <v>0.1</v>
+      </c>
+      <c r="D80">
+        <v>9.9999999999999384E+35</v>
       </c>
       <c r="E80">
-        <v>4.5080042116137202E-120</v>
+        <v>2.5192172068311015E+19</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>1.5460415516953768E+52</v>
       </c>
       <c r="G80">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>3.8948144795068494E+71</v>
       </c>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C81">
-        <v>1.0000000000000044E-75</v>
+        <v>0.1</v>
+      </c>
+      <c r="D81">
+        <v>3.1622776601683597E+36</v>
       </c>
       <c r="E81">
-        <v>8.9615047642627071E-122</v>
+        <v>3.4218582718973334E+19</v>
       </c>
       <c r="F81">
-        <v>-1.7486534454335398E+53</v>
+        <v>-1.1395768933873843E+53</v>
       </c>
       <c r="G81">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-3.8994706191006868E+72</v>
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C82">
-        <v>1.0000000000000044E-76</v>
+        <v>0.1</v>
+      </c>
+      <c r="D82">
+        <v>9.999999999999937E+36</v>
       </c>
       <c r="E82">
-        <v>1.7776401065825573E-123</v>
+        <v>4.6295192191470281E+19</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>-1.1554665171884528E+54</v>
       </c>
       <c r="G82">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-5.3492544484048222E+73</v>
       </c>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C83">
-        <v>1.0000000000000043E-77</v>
+        <v>0.1</v>
+      </c>
+      <c r="D83">
+        <v>3.1622776601683591E+37</v>
       </c>
       <c r="E83">
-        <v>3.518735908531554E-125</v>
+        <v>6.2389928472208933E+19</v>
       </c>
       <c r="F83">
-        <v>1.3114900840751548E+55</v>
+        <v>8.4312800486865378E+54</v>
       </c>
       <c r="G83">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>5.2602695916671538E+74</v>
       </c>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C84">
-        <v>1.0000000000000044E-78</v>
+        <v>0.1</v>
+      </c>
+      <c r="D84">
+        <v>9.9999999999999356E+37</v>
       </c>
       <c r="E84">
-        <v>6.9506068568149413E-127</v>
+        <v>8.3757609495641047E+19</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>8.8658583311191067E+55</v>
       </c>
       <c r="G84">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>7.4258309994155004E+75</v>
       </c>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C85">
-        <v>1.0000000000000045E-79</v>
+        <v>0.1</v>
+      </c>
+      <c r="D85">
+        <v>3.1622776601683588E+38</v>
       </c>
       <c r="E85">
-        <v>1.3701399251972104E-128</v>
+        <v>1.1201881213508772E+20</v>
       </c>
       <c r="F85">
-        <v>-1.0098473647378693E+57</v>
+        <v>-6.4034270541774427E+56</v>
       </c>
       <c r="G85">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-7.1730429220264107E+76</v>
       </c>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C86">
-        <v>1.0000000000000045E-80</v>
+        <v>0.1</v>
+      </c>
+      <c r="D86">
+        <v>9.9999999999999344E+38</v>
       </c>
       <c r="E86">
-        <v>2.6954162784958687E-130</v>
+        <v>1.4925866280327116E+20</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>-6.9794037688146771E+57</v>
       </c>
       <c r="G86">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-1.0417364736973897E+78</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C87">
-        <v>1.0000000000000045E-81</v>
+        <v>0.1</v>
+      </c>
+      <c r="D87">
+        <v>3.1622776601683581E+39</v>
       </c>
       <c r="E87">
-        <v>5.2919746018762234E-132</v>
+        <v>1.9815011178566582E+20</v>
       </c>
       <c r="F87">
-        <v>7.9777941814291672E+58</v>
+        <v>4.9889133351120333E+58</v>
       </c>
       <c r="G87">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>9.8855373504144831E+78</v>
       </c>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C88">
-        <v>1.0000000000000046E-82</v>
+        <v>0.1</v>
+      </c>
+      <c r="D88">
+        <v>9.9999999999999314E+39</v>
       </c>
       <c r="E88">
-        <v>1.0369374669029524E-133</v>
+        <v>2.6210718147801049E+20</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>5.6334121484028618E+59</v>
       </c>
       <c r="G88">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>1.4765577803218578E+80</v>
       </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C89">
-        <v>1.0000000000000048E-83</v>
+        <v>0.1</v>
+      </c>
+      <c r="D89">
+        <v>3.1622776601683572E+40</v>
       </c>
       <c r="E89">
-        <v>2.0278784468521844E-135</v>
+        <v>3.4547476869599357E+20</v>
       </c>
       <c r="F89">
-        <v>-6.4620132869576254E+60</v>
+        <v>-3.9846856799567184E+60</v>
       </c>
       <c r="G89">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-1.376608363609285E+81</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C90">
-        <v>1.0000000000000048E-84</v>
+        <v>0.1</v>
+      </c>
+      <c r="D90">
+        <v>9.9999999999999285E+40</v>
       </c>
       <c r="E90">
-        <v>3.9581945757335556E-137</v>
+        <v>4.5376285572355542E+20</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>-4.6592448184899135E+61</v>
       </c>
       <c r="G90">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-2.1141922343531618E+82</v>
       </c>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C91">
-        <v>1.0000000000000048E-85</v>
+        <v>0.1</v>
+      </c>
+      <c r="D91">
+        <v>3.1622776601683566E+41</v>
       </c>
       <c r="E91">
-        <v>7.7113297143786361E-139</v>
+        <v>5.9393446832697757E+20</v>
       </c>
       <c r="F91">
-        <v>5.3634710281748292E+62</v>
+        <v>3.2606966661791771E+62</v>
       </c>
       <c r="G91">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>1.9366401408026777E+83</v>
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C92">
-        <v>1.0000000000000049E-86</v>
+        <v>0.1</v>
+      </c>
+      <c r="D92">
+        <v>9.9999999999999277E+41</v>
       </c>
       <c r="E92">
-        <v>1.4995090518089781E-140</v>
+        <v>7.7475843810841251E+20</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>3.9463726141933186E+63</v>
       </c>
       <c r="G92">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>3.0574854827662282E+84</v>
       </c>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C93">
-        <v>1.0000000000000049E-87</v>
+        <v>0.1</v>
+      </c>
+      <c r="D93">
+        <v>3.1622776601683564E+42</v>
       </c>
       <c r="E93">
-        <v>2.9104966547481868E-142</v>
+        <v>1.0072400096910994E+21</v>
       </c>
       <c r="F93">
-        <v>-4.5589503739486049E+64</v>
+        <v>-2.7321284401103677E+64</v>
       </c>
       <c r="G93">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-2.7519090764940951E+85</v>
       </c>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C94">
-        <v>1.000000000000005E-88</v>
+        <v>0.1</v>
+      </c>
+      <c r="D94">
+        <v>9.9999999999999271E+42</v>
       </c>
       <c r="E94">
-        <v>5.6388892416643061E-144</v>
+        <v>1.3051446104021339E+21</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>-3.4212017326073579E+65</v>
       </c>
       <c r="G94">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-4.4651630024109358E+86</v>
       </c>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C95">
-        <v>1.0000000000000051E-89</v>
+        <v>0.1</v>
+      </c>
+      <c r="D95">
+        <v>3.1622776601683561E+43</v>
       </c>
       <c r="E95">
-        <v>1.0905321638402795E-145</v>
+        <v>1.6856327028843023E+21</v>
       </c>
       <c r="F95">
-        <v>3.9662868253352865E+66</v>
+        <v>2.3427397255699465E+66</v>
       </c>
       <c r="G95">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>3.9489986957668976E+87</v>
       </c>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C96">
-        <v>1.0000000000000052E-90</v>
+        <v>0.1</v>
+      </c>
+      <c r="D96">
+        <v>9.9999999999999256E+43</v>
       </c>
       <c r="E96">
-        <v>2.1052885055419015E-147</v>
+        <v>2.1700266020873833E+21</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>3.0340849219501741E+67</v>
       </c>
       <c r="G96">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>6.5840449936240996E+88</v>
       </c>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C97">
-        <v>1.0000000000000053E-91</v>
+        <v>0.1</v>
+      </c>
+      <c r="D97">
+        <v>3.1622776601683557E+44</v>
       </c>
       <c r="E97">
-        <v>4.0571636587974034E-149</v>
+        <v>2.7847334907196122E+21</v>
       </c>
       <c r="F97">
-        <v>-3.5299952745484048E+68</v>
+        <v>-2.0546975065377505E+68</v>
       </c>
       <c r="G97">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-5.7217849597537531E+89</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C98">
-        <v>1.0000000000000054E-92</v>
+        <v>0.1</v>
+      </c>
+      <c r="D98">
+        <v>9.9999999999999248E+44</v>
       </c>
       <c r="E98">
-        <v>7.8051368455929145E-151</v>
+        <v>3.5623526450014532E+21</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>-2.7512234048205342E+69</v>
       </c>
       <c r="G98">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-9.8008279731523336E+90</v>
       </c>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C99">
-        <v>1.0000000000000054E-93</v>
+        <v>0.1</v>
+      </c>
+      <c r="D99">
+        <v>3.1622776601683554E+45</v>
       </c>
       <c r="E99">
-        <v>1.498976110614955E-152</v>
+        <v>4.5429991184849484E+21</v>
       </c>
       <c r="F99">
-        <v>3.2122956998390481E+70</v>
+        <v>1.8422624969011475E+70</v>
       </c>
       <c r="G99">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>8.3693968994397936E+91</v>
       </c>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C100">
-        <v>1.0000000000000055E-94</v>
+        <v>0.1</v>
+      </c>
+      <c r="D100">
+        <v>9.9999999999999239E+45</v>
       </c>
       <c r="E100">
-        <v>2.8739155082862047E-154</v>
+        <v>5.7758808575420137E+21</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>2.5495481574039026E+71</v>
       </c>
       <c r="G100">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>1.4725886397730714E+93</v>
       </c>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C101">
-        <v>1.0000000000000056E-95</v>
+        <v>0.1</v>
+      </c>
+      <c r="D101">
+        <v>3.1622776601683544E+46</v>
       </c>
       <c r="E101">
-        <v>5.5008154615402773E-156</v>
+        <v>7.3211714674623408E+21</v>
       </c>
       <c r="F101">
-        <v>-2.9874350008503146E+72</v>
+        <v>-1.6878086405440281E+72</v>
       </c>
       <c r="G101">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-1.2356736461687341E+94</v>
       </c>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C102">
-        <v>1.0000000000000057E-96</v>
+        <v>0.1</v>
+      </c>
+      <c r="D102">
+        <v>9.9999999999999213E+46</v>
       </c>
       <c r="E102">
-        <v>1.0511445868045559E-157</v>
+        <v>9.252226639285824E+21</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>-2.4134533543651086E+73</v>
       </c>
       <c r="G102">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-2.2329817417930589E+95</v>
       </c>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C103">
-        <v>1.0000000000000058E-97</v>
+        <v>0.1</v>
+      </c>
+      <c r="D103">
+        <v>3.1622776601683542E+47</v>
       </c>
       <c r="E103">
-        <v>2.0053420631795109E-159</v>
+        <v>1.1658198606457963E+22</v>
       </c>
       <c r="F103">
-        <v>2.838063250807799E+74</v>
+        <v>1.5792836749731758E+74</v>
       </c>
       <c r="G103">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>1.8411602738774087E+96</v>
       </c>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C104">
-        <v>1.0000000000000058E-98</v>
+        <v>0.1</v>
+      </c>
+      <c r="D104">
+        <v>9.9999999999999193E+47</v>
       </c>
       <c r="E104">
-        <v>3.8195590727277021E-161</v>
+        <v>1.4647109943328451E+22</v>
       </c>
       <c r="F104">
-        <v>0</v>
+        <v>2.3327080569402361E+75</v>
       </c>
       <c r="G104">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>3.4167431375691722E+97</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C105">
-        <v>1.0000000000000059E-99</v>
+        <v>0.1</v>
+      </c>
+      <c r="D105">
+        <v>3.1622776601683533E+48</v>
       </c>
       <c r="E105">
-        <v>7.26347966823525E-163</v>
+        <v>1.83494555533973E+22</v>
       </c>
       <c r="F105">
-        <v>-2.7529213532835649E+76</v>
+        <v>-1.5085780841545783E+76</v>
       </c>
       <c r="G105">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-2.7681586504023684E+98</v>
       </c>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C106">
-        <v>1.000000000000006E-100</v>
+        <v>0.1</v>
+      </c>
+      <c r="D106">
+        <v>9.9999999999999177E+48</v>
       </c>
       <c r="E106">
-        <v>1.3790840638088982E-164</v>
+        <v>2.2922409824241242E+22</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>-2.3011396766429772E+77</v>
       </c>
       <c r="G106">
-        <f t="shared" si="1"/>
-        <v>0.99945219075983904</v>
+        <v>-5.2747666730832298E+99</v>
+      </c>
+    </row>
+    <row r="107" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="D107">
+        <v>3.1622776601683523E+49</v>
+      </c>
+    </row>
+    <row r="108" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="D108">
+        <v>9.9999999999999156E+49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove goofy __ class and _ member function for cumulants. Make scale a global function. More tests Remove scale from cumulants. Use class scale instead. Implement Excel versions.
</commit_message>
<xml_diff>
--- a/gop.xlsx
+++ b/gop.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\tmp\GR6250-2019\hw6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC61B29-DDC0-4FFB-AE07-F04034F24550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE187766-6A86-4A77-96FE-C76BFC49383D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{D3B39B31-0FCC-485C-968B-EB7A4BAB9E1D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Poisson" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>General Option Pricing</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>x_</t>
+  </si>
+  <si>
+    <t>pdf</t>
   </si>
 </sst>
 </file>
@@ -114,10 +117,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,1809 +439,1822 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0254B9-6FD0-4A8A-AD90-E09EBAA5AE26}">
-  <dimension ref="B2:L108"/>
+  <dimension ref="B2:J109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="E3" s="1" t="s">
+      <c r="E2" cm="1">
+        <f t="array" ref="E2">_xll.XLL.SEQUENCE.LIST({0,0})</f>
+        <v>30049430</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="E3" cm="1">
+        <f t="array" ref="E3">_xll.XLL.SEQUENCE.CONCATENATE(E2,D7)</f>
+        <v>-234210</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" cm="1">
-        <f t="array" ref="D4:D6">_xll.XLL.CUMULANT.NORMALIZE(C6)</f>
-        <v>0.1</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" cm="1">
+        <f t="array" ref="D5:D7">_xll.XLL.CUMULANT.NORMALIZE(C7)</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F4">
-        <f>(F3-D4)/D5</f>
+      <c r="F5">
+        <f>(F4-D5)/D6</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" cm="1">
+        <f t="array" ref="C7">_xll.XLL.CUMULANT.POISSON(C6,C5)</f>
+        <v>-357658</v>
+      </c>
+      <c r="D7">
+        <v>30389716</v>
+      </c>
+      <c r="E7" cm="1">
+        <f t="array" ref="E7">_xll.XLL.BELL.REDUCED(E3,1)</f>
+        <v>-212478</v>
+      </c>
+      <c r="F7" cm="1">
+        <f t="array" ref="F7">_xll.XLL.HERMITE(F5)</f>
+        <v>78209912</v>
+      </c>
+      <c r="G7" cm="1">
+        <f t="array" ref="G7">_xll.XLL.SEQUENCE.MUL(E7,F7)</f>
+        <v>-234084</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8" cm="1">
+        <f t="array" ref="C8:C107">_xll.XLL.SEQUENCE.TAKE(B8,C7)</f>
+        <v>1</v>
+      </c>
+      <c r="E8" cm="1">
+        <f t="array" ref="E8:E107">_xll.XLL.SEQUENCE.TAKE(B8,E7)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" cm="1">
+        <f t="array" ref="F8:F107">_xll.XLL.SEQUENCE.TAKE(B8,F7)</f>
+        <v>1</v>
+      </c>
+      <c r="G8" cm="1">
+        <f t="array" ref="G8:G107">_xll.XLL.SEQUENCE.TAKE(B8,G7)</f>
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>0.1</v>
-      </c>
-      <c r="D5">
-        <v>0.31622776601683794</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" cm="1">
-        <f t="array" ref="C6">_xll.XLL.CUMULANT.POISSON(C5,C4)</f>
-        <v>29179580</v>
-      </c>
-      <c r="D6">
-        <v>28651638</v>
-      </c>
-      <c r="E6" cm="1">
-        <f t="array" ref="E6">_xll.XLL.BELL.REDUCED(D6,{1,0,0})</f>
-        <v>30145922</v>
-      </c>
-      <c r="F6" cm="1">
-        <f t="array" ref="F6">_xll.XLL.HERMITE(F3)</f>
-        <v>-1365472</v>
-      </c>
-      <c r="G6" cm="1">
-        <f t="array" ref="G6">_xll.XLL.SEQUENCE.MUL(E6,F6)</f>
-        <v>29657044</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="C7" cm="1">
-        <f t="array" ref="C7:C106">_xll.XLL.SEQUENCE.TAKE(B7,C6)</f>
-        <v>0.1</v>
-      </c>
-      <c r="E7" cm="1">
-        <f t="array" ref="E7:E106">_xll.XLL.SEQUENCE.TAKE(B7,E6)</f>
-        <v>1</v>
-      </c>
-      <c r="F7" cm="1">
-        <f t="array" ref="F7:F106">_xll.XLL.SEQUENCE.TAKE(B7,F6)</f>
-        <v>1</v>
-      </c>
-      <c r="G7" cm="1">
-        <f t="array" ref="G7:G106">_xll.XLL.SEQUENCE.TAKE(B7,G6)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="C8">
-        <v>0.1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0.1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="J8" cm="1">
+        <f t="array" ref="J8">_xll.XLL.OPTION.PDF(F4, $C$7)</f>
+        <v>-9.9227215334176043E+32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C9">
-        <v>0.1</v>
-      </c>
-      <c r="D9" cm="1">
-        <f t="array" ref="D9:D108">_xll.XLL.SEQUENCE.TAKE(B7,D6)</f>
-        <v>3.1622776601683791</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>-0.99</v>
+        <v>-1</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C10">
-        <v>0.1</v>
-      </c>
-      <c r="D10">
-        <v>9.9999999999999982</v>
+        <v>1</v>
+      </c>
+      <c r="D10" cm="1">
+        <f t="array" ref="D10:D109">_xll.XLL.SEQUENCE.TAKE(B8,D7)</f>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>16.666666666666661</v>
+        <v>0.5</v>
       </c>
       <c r="F10">
-        <v>-0.29900000000000004</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>-4.9833333333333325</v>
-      </c>
-      <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" cm="1">
-        <f t="array" ref="L10">_xll.XLL.OPTION.PDF(F3, $C$6)</f>
-        <v>-77.5003130223743</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C11">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>31.622776601683785</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>54.842823584034882</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F11">
-        <v>2.9400999999999997</v>
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>161.24338561942093</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C12">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>99.999999999999972</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>223.428235840349</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F12">
-        <v>1.4900100000000003</v>
+        <v>-2</v>
       </c>
       <c r="G12">
-        <v>332.91030568447849</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C13">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>316.22776601683779</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>804.70839399584145</v>
+        <v>9.166666666666666E-2</v>
       </c>
       <c r="F13">
-        <v>-14.551498999999998</v>
+        <v>-6</v>
       </c>
       <c r="G13">
-        <v>-11709.713390522091</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-0.54999999999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C14">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>999.99999999999943</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>2678.1350939563722</v>
+        <v>5.6944444444444443E-2</v>
       </c>
       <c r="F14">
-        <v>-10.395209900000003</v>
+        <v>16</v>
       </c>
       <c r="G14">
-        <v>-27839.77644223272</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+        <v>0.91111111111111109</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>3162.2776601683772</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>8373.8832383289791</v>
+        <v>3.2142857142857147E-2</v>
       </c>
       <c r="F15">
-        <v>100.82097200999999</v>
+        <v>20</v>
       </c>
       <c r="G15">
-        <v>844263.0475865741</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+        <v>0.6428571428571429</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C16">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>9999.9999999999927</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>24796.313876427808</v>
+        <v>1.773313492063492E-2</v>
       </c>
       <c r="F16">
-        <v>93.243776401000019</v>
+        <v>-132</v>
       </c>
       <c r="G16">
-        <v>2312101.9466626486</v>
+        <v>-2.3407738095238093</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C17">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>31622.776601683767</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>70007.428673019051</v>
+        <v>9.4383818342151683E-3</v>
       </c>
       <c r="F17">
-        <v>-898.06437044989991</v>
+        <v>-28</v>
       </c>
       <c r="G17">
-        <v>-62871177.358051129</v>
+        <v>-0.26427469135802473</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C18">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>99999.999999999927</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>189484.61612898347</v>
+        <v>4.8837081128747803E-3</v>
       </c>
       <c r="F18">
-        <v>-1022.2442010549901</v>
+        <v>1216</v>
       </c>
       <c r="G18">
-        <v>-193699550.02698418</v>
+        <v>5.9385890652557327</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C19">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>316227.76601683762</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>493843.09249147674</v>
+        <v>2.4614448051948059E-3</v>
       </c>
       <c r="F19">
-        <v>9776.4836548434014</v>
+        <v>-936</v>
       </c>
       <c r="G19">
-        <v>4828048921.8002405</v>
+        <v>-2.3039123376623385</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C20">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>999999.99999999895</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>1243840.6408390945</v>
+        <v>1.2115136984928653E-3</v>
       </c>
       <c r="F20">
-        <v>13244.57877814422</v>
+        <v>-12440</v>
       </c>
       <c r="G20">
-        <v>16474145355.050777</v>
+        <v>-15.071230409251244</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C21">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>3162277.6601683758</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>3036838.9492958165</v>
+        <v>5.8347002791447238E-4</v>
       </c>
       <c r="F21">
-        <v>-125769.8296351498</v>
+        <v>23672</v>
       </c>
       <c r="G21">
-        <v>-381942717282.32214</v>
+        <v>13.81190250079139</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C22">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>9999999.9999999888</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>7205779.0583372582</v>
+        <v>2.7542587345414737E-4</v>
       </c>
       <c r="F22">
-        <v>-198001.08585753405</v>
+        <v>138048</v>
       </c>
       <c r="G22">
-        <v>-1426752078000.2563</v>
+        <v>38.02199097859814</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C23">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>31622776.601683758</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>16653457.025567412</v>
+        <v>1.2762211226579614E-4</v>
       </c>
       <c r="F23">
-        <v>1866747.3359414935</v>
+        <v>-469456</v>
       </c>
       <c r="G23">
-        <v>31087796536694.117</v>
+        <v>-59.912966335851593</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C24">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>99999999.999999866</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>37560048.238612562</v>
+        <v>5.8121808157977159E-5</v>
       </c>
       <c r="F24">
-        <v>3354692.1073146942</v>
+        <v>-1601264</v>
       </c>
       <c r="G24">
-        <v>126002397376432.75</v>
+        <v>-93.068359018275132</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C25">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>316227766.01683748</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>82808591.088176101</v>
+        <v>2.6045541774109681E-5</v>
       </c>
       <c r="F25">
-        <v>-31399235.500273921</v>
+        <v>9112560</v>
       </c>
       <c r="G25">
-        <v>-2600126453023525.5</v>
+        <v>237.34156214908091</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C26">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>999999999.99999845</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>178728858.77149701</v>
+        <v>1.1495860975930179E-5</v>
       </c>
       <c r="F26">
-        <v>-63524381.481691889</v>
+        <v>18108928</v>
       </c>
       <c r="G26">
-        <v>-1.135364020638801E+16</v>
+        <v>208.17771871112936</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C27">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>3162277660.1683741</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>378141199.27136135</v>
+        <v>5.002059319092985E-6</v>
       </c>
       <c r="F27">
-        <v>590233036.35703528</v>
+        <v>-182135008</v>
       </c>
       <c r="G27">
-        <v>2.2319142821762634E+17</v>
+        <v>-911.05011409947542</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C28">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>9999999999.9999828</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>785167127.3641845</v>
+        <v>2.1473393418135951E-6</v>
       </c>
       <c r="F28">
-        <v>1329510933.2695413</v>
+        <v>-161934624</v>
       </c>
       <c r="G28">
-        <v>1.0438882802745217E+18</v>
+        <v>-347.72858891699201</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C29">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>31622776601.683735</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>1601679639.4255438</v>
+        <v>9.1013964632238371E-7</v>
       </c>
       <c r="F29">
-        <v>-12261942670.170788</v>
+        <v>3804634784</v>
       </c>
       <c r="G29">
-        <v>-1.9639703914615837E+19</v>
+        <v>3462.7489566955987</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C30">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>99999999999.999802</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>3212969098.2472124</v>
+        <v>3.811117853680523E-7</v>
       </c>
       <c r="F30">
-        <v>-30475434798.946987</v>
+        <v>-404007680</v>
       </c>
       <c r="G30">
-        <v>-9.7916630264664424E+19</v>
+        <v>-153.97208822720475</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C31">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D31">
-        <v>316227766016.83728</v>
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>6343487121.283843</v>
+        <v>1.5775735624503972E-7</v>
       </c>
       <c r="F31">
-        <v>278977137934.03339</v>
+        <v>-83297957568</v>
       </c>
       <c r="G31">
-        <v>1.7696878816171671E+21</v>
+        <v>-13140.865566539178</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C32">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>999999999999.9978</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>12336156583.07688</v>
+        <v>6.4588223499018579E-8</v>
       </c>
       <c r="F32">
-        <v>759308148968.13098</v>
+        <v>92590134208</v>
       </c>
       <c r="G32">
-        <v>9.3669442204771287E+21</v>
+        <v>5980.2322820304298</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C33">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>3162277660168.3721</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>23646794500.094364</v>
+        <v>2.6167217652278485E-8</v>
       </c>
       <c r="F33">
-        <v>-6898497633454.0215</v>
+        <v>1906560847424</v>
       </c>
       <c r="G33">
-        <v>-1.6312735589767454E+23</v>
+        <v>49889.39266185632</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C34">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D34">
-        <v>9999999999999.9766</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>44708462874.090202</v>
+        <v>1.0495399806263624E-8</v>
       </c>
       <c r="F34">
-        <v>-20431861636516.809</v>
+        <v>-4221314202624</v>
       </c>
       <c r="G34">
-        <v>-9.1347712742475957E+23</v>
+        <v>-44304.380264397812</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C35">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D35">
-        <v>31622776601683.715</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>83424554661.785324</v>
+        <v>4.1692612449218577E-9</v>
       </c>
       <c r="F35">
-        <v>184216249939606.91</v>
+        <v>-45349267830400</v>
       </c>
       <c r="G35">
-        <v>1.5368158612675845E+25</v>
+        <v>-189072.94485086825</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C36">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>99999999999999.734</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>153718497770.65823</v>
+        <v>1.6409892846923698E-9</v>
       </c>
       <c r="F36">
-        <v>590513750816431.38</v>
+        <v>159324751301248</v>
       </c>
       <c r="G36">
-        <v>9.077288668841863E+25</v>
+        <v>261450.20967162467</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C37">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>316227766016837.13</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>279839980237.88007</v>
+        <v>6.4016888286205427E-10</v>
       </c>
       <c r="F37">
-        <v>-5283219873166957</v>
+        <v>1110454747949952</v>
       </c>
       <c r="G37">
-        <v>-1.4784561448994165E+27</v>
+        <v>710878.57546398486</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C38">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D38">
-        <v>999999999999997.5</v>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>503560831538.18988</v>
+        <v>2.4761120798961171E-10</v>
       </c>
       <c r="F38">
-        <v>-1.8243734511809636E+16</v>
+        <v>-5730872535686144</v>
       </c>
       <c r="G38">
-        <v>-9.1868301211288328E+27</v>
+        <v>-1419028.2713957352</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C39">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D39">
-        <v>3162277660168371</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>896076957629.67297</v>
+        <v>9.4987809723611869E-11</v>
       </c>
       <c r="F39">
-        <v>1.6195544261699472E+17</v>
+        <v>-2.7582769902812416E+16</v>
       </c>
       <c r="G39">
-        <v>1.4512454029180372E+29</v>
+        <v>-2620026.8991785143</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C40">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D40">
-        <v>9999999999999972</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>1577500165472.9888</v>
+        <v>3.6150417121777208E-11</v>
       </c>
       <c r="F40">
-        <v>5.9999504863960781E+17</v>
+        <v>2.0523981850908288E+17</v>
       </c>
       <c r="G40">
-        <v>9.4649228851195521E+29</v>
+        <v>7419505.0491011962</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C41">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <v>3.1622776601683704E+16</v>
+        <v>1</v>
       </c>
       <c r="E41">
-        <v>2748476114928.8667</v>
+        <v>1.36528900290733E-11</v>
       </c>
       <c r="F41">
-        <v>-5.2845301014968648E+18</v>
+        <v>6.7740881838091443E+17</v>
       </c>
       <c r="G41">
-        <v>-1.4524404762586752E+31</v>
+        <v>9248588.1020791121</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C42">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>9.9999999999999712E+16</v>
+        <v>1</v>
       </c>
       <c r="E42">
-        <v>4740999934010.7979</v>
+        <v>5.1181424192172987E-12</v>
       </c>
       <c r="F42">
-        <v>-2.0928284663896351E+19</v>
+        <v>-7.4503228291806495E+18</v>
       </c>
       <c r="G42">
-        <v>-9.9220996210491799E+31</v>
+        <v>-38131813.308892518</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C43">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D43">
-        <v>3.1622776601683699E+17</v>
+        <v>1</v>
       </c>
       <c r="E43">
-        <v>8099357568166.1182</v>
+        <v>1.9049369989052495E-12</v>
       </c>
       <c r="F43">
-        <v>1.8286572508600061E+20</v>
+        <v>-1.5581576995770442E+19</v>
       </c>
       <c r="G43">
-        <v>1.4810948944334837E+33</v>
+        <v>-29681922.52053402</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C44">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D44">
-        <v>9.9999999999999693E+17</v>
+        <v>1</v>
       </c>
       <c r="E44">
-        <v>13707938325515.389</v>
+        <v>7.0408845611135607E-13</v>
       </c>
       <c r="F44">
-        <v>7.7170482040886867E+20</v>
+        <v>2.7634287601709315E+20</v>
       </c>
       <c r="G44">
-        <v>1.0578482083667701E+34</v>
+        <v>194569828.93224701</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C45">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D45">
-        <v>3.1622776601683692E+18</v>
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>22991368176201.898</v>
+        <v>2.584904349250129E-13</v>
       </c>
       <c r="F45">
-        <v>-6.6888613461411349E+21</v>
+        <v>2.8459389583064272E+20</v>
       </c>
       <c r="G45">
-        <v>-1.5378607388869629E+35</v>
+        <v>73564799.910266653</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C46">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>9.9999999999999672E+18</v>
+        <v>1</v>
       </c>
       <c r="E46">
-        <v>38225333861243.734</v>
+        <v>9.4279991034895734E-14</v>
       </c>
       <c r="F46">
-        <v>-2.9993669310151123E+22</v>
+        <v>-1.0509280308463091E+22</v>
       </c>
       <c r="G46">
-        <v>-1.1465180231042667E+36</v>
+        <v>-990814853.26510644</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C47">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>3.1622776601683685E+19</v>
+        <v>1</v>
       </c>
       <c r="E47">
-        <v>63015499904310.922</v>
+        <v>3.4169200588344151E-14</v>
       </c>
       <c r="F47">
-        <v>2.5786622556848913E+23</v>
+        <v>-3.0528773310133358E+20</v>
       </c>
       <c r="G47">
-        <v>1.6249569112636145E+37</v>
+        <v>-10431437.789500339</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C48">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D48">
-        <v>9.999999999999964E+19</v>
+        <v>1</v>
       </c>
       <c r="E48">
-        <v>103029745116261.64</v>
+        <v>1.2307459135207634E-14</v>
       </c>
       <c r="F48">
-        <v>1.2255333949628937E+24</v>
+        <v>4.1016721976316186E+23</v>
       </c>
       <c r="G48">
-        <v>1.2626639331449374E+38</v>
+        <v>5048116295.8368435</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C49">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <v>3.1622776601683683E+20</v>
+        <v>1</v>
       </c>
       <c r="E49">
-        <v>167109327020735.06</v>
+        <v>4.4065055560506948E-15</v>
       </c>
       <c r="F49">
-        <v>-1.0449961908811764E+25</v>
+        <v>-3.9795571043910849E+23</v>
       </c>
       <c r="G49">
-        <v>-1.7462861019738498E+39</v>
+        <v>-1753594049.1120331</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C50">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D50">
-        <v>9.9999999999999646E+20</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>268942771260570.13</v>
+        <v>1.5684940695349933E-15</v>
       </c>
       <c r="F50">
-        <v>-5.2517398779322711E+25</v>
+        <v>-1.6418900299850528E+25</v>
       </c>
       <c r="G50">
-        <v>-1.4124174767107533E+40</v>
+        <v>-25752947748.601879</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C51">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>3.1622776601683679E+21</v>
+        <v>1</v>
       </c>
       <c r="E51">
-        <v>429569546802828.94</v>
+        <v>5.5513795247958463E-16</v>
       </c>
       <c r="F51">
-        <v>4.4409662220097358E+26</v>
+        <v>3.3133040138293083E+25</v>
       </c>
       <c r="G51">
-        <v>1.9077038473553938E+41</v>
+        <v>18393408061.795914</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C52">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D52">
-        <v>9.9999999999999623E+21</v>
+        <v>1</v>
       </c>
       <c r="E52">
-        <v>681098921469461.38</v>
+        <v>1.9539437516010164E-16</v>
       </c>
       <c r="F52">
-        <v>2.3551752085102968E+27</v>
+        <v>6.7287967275527953E+26</v>
       </c>
       <c r="G52">
-        <v>1.604107294387977E+42</v>
+        <v>131476903215.95151</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C53">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D53">
-        <v>3.1622776601683671E+22</v>
+        <v>1</v>
       </c>
       <c r="E53">
-        <v>1072196447850081.4</v>
+        <v>6.840327871212992E-17</v>
       </c>
       <c r="F53">
-        <v>-1.9748830478192784E+28</v>
+        <v>-2.1307334388401752E+27</v>
       </c>
       <c r="G53">
-        <v>-2.1174625887911728E+43</v>
+        <v>-145749153278.23953</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C54">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D54">
-        <v>9.9999999999999589E+22</v>
+        <v>1</v>
       </c>
       <c r="E54">
-        <v>1676124831206619</v>
+        <v>2.3820634843791345E-17</v>
       </c>
       <c r="F54">
-        <v>-1.1031294263929292E+29</v>
+        <v>-2.8148851835147404E+28</v>
       </c>
       <c r="G54">
-        <v>-1.848982623611903E+44</v>
+        <v>-670523520837.03223</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C55">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D55">
-        <v>3.1622776601683666E+23</v>
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>2602452451415247.5</v>
+        <v>8.2527086649715804E-18</v>
       </c>
       <c r="F55">
-        <v>9.1716373821113162E+29</v>
+        <v>1.2616259002179546E+29</v>
       </c>
       <c r="G55">
-        <v>2.3868750188567317E+45</v>
+        <v>1041183099868.1284</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C56">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D56">
-        <v>9.9999999999999582E+23</v>
+        <v>1</v>
       </c>
       <c r="E56">
-        <v>4013995002609410</v>
+        <v>2.8448491511826437E-18</v>
       </c>
       <c r="F56">
-        <v>5.3867376205071732E+30</v>
+        <v>1.1968334462301325E+30</v>
       </c>
       <c r="G56">
-        <v>2.1622337889083899E+46</v>
+        <v>3404810613614.7905</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C57">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D57">
-        <v>3.1622776601683656E+24</v>
+        <v>1</v>
       </c>
       <c r="E57">
-        <v>6151178107493286</v>
+        <v>9.7587009273943784E-19</v>
       </c>
       <c r="F57">
-        <v>-4.4402349410294729E+31</v>
+        <v>-7.2526377672763149E+30</v>
       </c>
       <c r="G57">
-        <v>-2.7312675961387234E+47</v>
+        <v>-7077632290557.4863</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C58">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D58">
-        <v>9.9999999999999558E+24</v>
+        <v>1</v>
       </c>
       <c r="E58">
-        <v>9366860270486912</v>
+        <v>3.3315256214627825E-19</v>
       </c>
       <c r="F58">
-        <v>-2.7377711596638814E+32</v>
+        <v>-5.1392201098000179E+31</v>
       </c>
       <c r="G58">
-        <v>-2.5644319905140492E+48</v>
+        <v>-17121443470135.533</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C59">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D59">
-        <v>3.1622776601683653E+25</v>
+        <v>1</v>
       </c>
       <c r="E59">
-        <v>1.4175813620431232E+16</v>
+        <v>1.1320328332271736E-19</v>
       </c>
       <c r="F59">
-        <v>2.2371421083283923E+33</v>
+        <v>4.1402408946181593E+32</v>
       </c>
       <c r="G59">
-        <v>3.1713309570081865E+49</v>
+        <v>46868886301776.023</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C60">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D60">
-        <v>9.9999999999999524E+25</v>
+        <v>1</v>
       </c>
       <c r="E60">
-        <v>2.1324625811508404E+16</v>
+        <v>3.8289883545754878E-20</v>
       </c>
       <c r="F60">
-        <v>1.4460124241085023E+34</v>
+        <v>2.2069781665361934E+33</v>
       </c>
       <c r="G60">
-        <v>3.0835673862906005E+50</v>
+        <v>84504936984694.453</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C61">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D61">
-        <v>3.1622776601683645E+26</v>
+        <v>1</v>
       </c>
       <c r="E61">
-        <v>3.1889891760771748E+16</v>
+        <v>1.2893204849686693E-20</v>
       </c>
       <c r="F61">
-        <v>-1.1712251931729629E+35</v>
+        <v>-2.373623081855062E+34</v>
       </c>
       <c r="G61">
-        <v>-3.7350244637774771E+51</v>
+        <v>-306036086303019.56</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C62">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D62">
-        <v>9.999999999999952E+26</v>
+        <v>1</v>
       </c>
       <c r="E62">
-        <v>4.7415378546113E+16</v>
+        <v>4.3224553393739433E-21</v>
       </c>
       <c r="F62">
-        <v>-7.9255896095032091E+35</v>
+        <v>-9.3233612007867632E+34</v>
       </c>
       <c r="G62">
-        <v>-3.7579483153573455E+52</v>
+        <v>-402998124032526.06</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C63">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D63">
-        <v>3.1622776601683634E+27</v>
+        <v>1</v>
       </c>
       <c r="E63">
-        <v>7.0102589029275824E+16</v>
+        <v>1.4428870528709456E-21</v>
       </c>
       <c r="F63">
-        <v>6.3624826663562634E+36</v>
+        <v>1.3749900762096012E+36</v>
       </c>
       <c r="G63">
-        <v>4.4602650756546416E+53</v>
+        <v>1983955378788868.3</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C64">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D64">
-        <v>9.9999999999999512E+27</v>
+        <v>1</v>
       </c>
       <c r="E64">
-        <v>1.030740983169431E+17</v>
+        <v>4.7962768956328057E-22</v>
       </c>
       <c r="F64">
-        <v>4.5019550079853601E+37</v>
+        <v>3.7528585842231185E+36</v>
       </c>
       <c r="G64">
-        <v>4.640349531115374E+54</v>
+        <v>1799974892008658.5</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C65">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D65">
-        <v>3.1622776601683636E+28</v>
+        <v>1</v>
       </c>
       <c r="E65">
-        <v>1.5073554592695907E+17</v>
+        <v>1.5877522371074455E-22</v>
       </c>
       <c r="F65">
-        <v>-3.5815955697432162E+38</v>
+        <v>-8.0752302851960782E+37</v>
       </c>
       <c r="G65">
-        <v>-5.3987376349482176E+55</v>
+        <v>-1.2821464950477868E+16</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C66">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D66">
-        <v>9.9999999999999499E+28</v>
+        <v>1</v>
       </c>
       <c r="E66">
-        <v>2.1927068233617334E+17</v>
+        <v>5.2348343180501523E-23</v>
       </c>
       <c r="F66">
-        <v>-2.646949860328941E+39</v>
+        <v>-1.3316063644875697E+38</v>
       </c>
       <c r="G66">
-        <v>-5.8039850198396561E+56</v>
+        <v>-6970738694953529</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C67">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D67">
-        <v>3.1622776601683636E+29</v>
+        <v>1</v>
       </c>
       <c r="E67">
-        <v>3.1731495253310502E+17</v>
+        <v>1.7190905372971058E-23</v>
       </c>
       <c r="F67">
-        <v>2.0866718875452082E+40</v>
+        <v>4.8167942018624827E+39</v>
       </c>
       <c r="G67">
-        <v>6.6213219094857246E+57</v>
+        <v>8.28050533252936E+16</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C68">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D68">
-        <v>9.9999999999999481E+29</v>
+        <v>1</v>
       </c>
       <c r="E68">
-        <v>4.5686745191394464E+17</v>
+        <v>5.6234499987280985E-24</v>
       </c>
       <c r="F68">
-        <v>1.6090366350728168E+41</v>
+        <v>3.0396833486141785E+39</v>
       </c>
       <c r="G68">
-        <v>7.3511646750190543E+58</v>
+        <v>1.7093507322898224E+16</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C69">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D69">
-        <v>3.1622776601683627E+30</v>
+        <v>1</v>
       </c>
       <c r="E69">
-        <v>6.5451958143841587E+17</v>
+        <v>1.8325116445997474E-24</v>
       </c>
       <c r="F69">
-        <v>-1.2567794850518488E+42</v>
+        <v>-2.9204733546036315E+41</v>
       </c>
       <c r="G69">
-        <v>-8.2258678251652392E+59</v>
+        <v>-5.3518014300544422E+17</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C70">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D70">
-        <v>9.9999999999999467E+30</v>
+        <v>1</v>
       </c>
       <c r="E70">
-        <v>9.3310243405631642E+17</v>
+        <v>5.9492321979871585E-25</v>
       </c>
       <c r="F70">
-        <v>-1.0101705085956649E+43</v>
+        <v>1.0662665119489825E+41</v>
       </c>
       <c r="G70">
-        <v>-9.4259256038252208E+60</v>
+        <v>6.3434670645223456E+16</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C71">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D71">
-        <v>3.1622776601683627E+31</v>
+        <v>1</v>
       </c>
       <c r="E71">
-        <v>1.3238851831235328E+18</v>
+        <v>1.9243089219293337E-25</v>
       </c>
       <c r="F71">
-        <v>7.8166937049670814E+43</v>
+        <v>1.8000308147347617E+43</v>
       </c>
       <c r="G71">
-        <v>1.034840497702091E+62</v>
+        <v>3.4638153565418296E+18</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C72">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D72">
-        <v>9.9999999999999447E+31</v>
+        <v>1</v>
       </c>
       <c r="E72">
-        <v>1.8694951286661445E+18</v>
+        <v>6.2017864864721273E-26</v>
       </c>
       <c r="F72">
-        <v>6.5432581920619258E+44</v>
+        <v>-2.4717787172626206E+43</v>
       </c>
       <c r="G72">
-        <v>1.2232589315664615E+63</v>
+        <v>-1.5329443846268728E+18</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C73">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D73">
-        <v>3.1622776601683615E+32</v>
+        <v>1</v>
       </c>
       <c r="E73">
-        <v>2.6277785487179576E+18</v>
+        <v>1.991656713751253E-26</v>
       </c>
       <c r="F73">
-        <v>-5.0154183263079837E+45</v>
+        <v>-1.1273019342576212E+45</v>
       </c>
       <c r="G73">
-        <v>-1.3179408690719041E+64</v>
+        <v>-2.2451984657889649E+19</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C74">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D74">
-        <v>9.9999999999999447E+32</v>
+        <v>1</v>
       </c>
       <c r="E74">
-        <v>3.6768824690998892E+18</v>
+        <v>6.3737414452572667E-27</v>
       </c>
       <c r="F74">
-        <v>-4.3687045900239509E+46</v>
+        <v>2.7339581004783245E+45</v>
       </c>
       <c r="G74">
-        <v>-1.6063213319735283E+65</v>
+        <v>1.7425542054615527E+19</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C75">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D75">
-        <v>3.1622776601683613E+33</v>
+        <v>1</v>
       </c>
       <c r="E75">
-        <v>5.1219137529996503E+18</v>
+        <v>2.0327429429399904E-27</v>
       </c>
       <c r="F75">
-        <v>3.3166432327261096E+47</v>
+        <v>7.1667969560524677E+46</v>
       </c>
       <c r="G75">
-        <v>1.698756058749308E+66</v>
+        <v>1.4568255935899458E+20</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C76">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D76">
-        <v>9.9999999999999418E+33</v>
+        <v>1</v>
       </c>
       <c r="E76">
-        <v>7.1036269252511805E+18</v>
+        <v>6.4610561564248511E-28</v>
       </c>
       <c r="F76">
-        <v>3.0038855535435478E+48</v>
+        <v>-2.5484316229257242E+47</v>
       </c>
       <c r="G76">
-        <v>2.1338482298524992E+67</v>
+        <v>-1.6465559826532024E+20</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C77">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D77">
-        <v>3.1622776601683613E+34</v>
+        <v>1</v>
       </c>
       <c r="E77">
-        <v>9.8097099323040113E+18</v>
+        <v>2.0468301393964048E-28</v>
       </c>
       <c r="F77">
-        <v>-2.2584449750455802E+49</v>
+        <v>-4.6185787678231058E+48</v>
       </c>
       <c r="G77">
-        <v>-2.2154690103266712E+68</v>
+        <v>-9.4534462231566431E+20</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C78">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D78">
-        <v>9.9999999999999407E+34</v>
+        <v>1</v>
       </c>
       <c r="E78">
-        <v>1.3489382383018002E+19</v>
+        <v>6.4630986932531195E-29</v>
       </c>
       <c r="F78">
-        <v>-2.1253043372309395E+50</v>
+        <v>2.2202756966010601E+49</v>
       </c>
       <c r="G78">
-        <v>-2.8669042885194786E+69</v>
+        <v>1.4349860953363972E+21</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C79">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D79">
-        <v>3.1622776601683603E+35</v>
+        <v>1</v>
       </c>
       <c r="E79">
-        <v>1.8472199345134035E+19</v>
+        <v>2.0342448618725924E-29</v>
       </c>
       <c r="F79">
-        <v>1.5822428889100523E+51</v>
+        <v>3.0109775678160684E+50</v>
       </c>
       <c r="G79">
-        <v>2.9227506056367251E+70</v>
+        <v>6.1250656465434727E+21</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C80">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D80">
-        <v>9.9999999999999384E+35</v>
+        <v>1</v>
       </c>
       <c r="E80">
-        <v>2.5192172068311015E+19</v>
+        <v>6.3825056476488771E-30</v>
       </c>
       <c r="F80">
-        <v>1.5460415516953768E+52</v>
+        <v>-1.8774935013683595E+51</v>
       </c>
       <c r="G80">
-        <v>3.8948144795068494E+71</v>
+        <v>-1.198311287590762E+22</v>
       </c>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C81">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D81">
-        <v>3.1622776601683597E+36</v>
+        <v>1</v>
       </c>
       <c r="E81">
-        <v>3.4218582718973334E+19</v>
+        <v>1.9963016576425692E-30</v>
       </c>
       <c r="F81">
-        <v>-1.1395768933873843E+53</v>
+        <v>-1.9801544986907332E+52</v>
       </c>
       <c r="G81">
-        <v>-3.8994706191006868E+72</v>
+        <v>-3.9529857081247015E+22</v>
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C82">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D82">
-        <v>9.999999999999937E+36</v>
+        <v>1</v>
       </c>
       <c r="E82">
-        <v>4.6295192191470281E+19</v>
+        <v>6.2248505367896824E-31</v>
       </c>
       <c r="F82">
-        <v>-1.1554665171884528E+54</v>
+        <v>1.5685857058679757E+53</v>
       </c>
       <c r="G82">
-        <v>-5.3492544484048222E+73</v>
+        <v>9.7642115731728921E+22</v>
       </c>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C83">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D83">
-        <v>3.1622776601683591E+37</v>
+        <v>1</v>
       </c>
       <c r="E83">
-        <v>6.2389928472208933E+19</v>
+        <v>1.9351726591756483E-31</v>
       </c>
       <c r="F83">
-        <v>8.4312800486865378E+54</v>
+        <v>1.308455758444345E+54</v>
       </c>
       <c r="G83">
-        <v>5.2602695916671538E+74</v>
+        <v>2.5320878094824328E+23</v>
       </c>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C84">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D84">
-        <v>9.9999999999999356E+37</v>
+        <v>1</v>
       </c>
       <c r="E84">
-        <v>8.3757609495641047E+19</v>
+        <v>5.9981621651517076E-32</v>
       </c>
       <c r="F84">
-        <v>8.8658583311191067E+55</v>
+        <v>-1.3072848552454163E+55</v>
       </c>
       <c r="G84">
-        <v>7.4258309994155004E+75</v>
+        <v>-7.8413065578088823E+23</v>
       </c>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C85">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D85">
-        <v>3.1622776601683588E+38</v>
+        <v>1</v>
       </c>
       <c r="E85">
-        <v>1.1201881213508772E+20</v>
+        <v>1.8537172685336726E-32</v>
       </c>
       <c r="F85">
-        <v>-6.4034270541774427E+56</v>
+        <v>-8.6369789089316068E+55</v>
       </c>
       <c r="G85">
-        <v>-7.1730429220264107E+76</v>
+        <v>-1.6010516951447639E+24</v>
       </c>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C86">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D86">
-        <v>9.9999999999999344E+38</v>
+        <v>1</v>
       </c>
       <c r="E86">
-        <v>1.4925866280327116E+20</v>
+        <v>5.7123418722442508E-33</v>
       </c>
       <c r="F86">
-        <v>-6.9794037688146771E+57</v>
+        <v>1.0929791276282867E+57</v>
       </c>
       <c r="G86">
-        <v>-1.0417364736973897E+78</v>
+        <v>6.2434704362400552E+24</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C87">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D87">
-        <v>3.1622776601683581E+39</v>
+        <v>1</v>
       </c>
       <c r="E87">
-        <v>1.9815011178566582E+20</v>
+        <v>1.7552879899260066E-33</v>
       </c>
       <c r="F87">
-        <v>4.9889133351120333E+58</v>
+        <v>5.6438644213383661E+57</v>
       </c>
       <c r="G87">
-        <v>9.8855373504144831E+78</v>
+        <v>9.906607435545925E+24</v>
       </c>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C88">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D88">
-        <v>9.9999999999999314E+39</v>
+        <v>1</v>
       </c>
       <c r="E88">
-        <v>2.6210718147801049E+20</v>
+        <v>5.3785309862300318E-34</v>
       </c>
       <c r="F88">
-        <v>5.6334121484028618E+59</v>
+        <v>-9.198921550397302E+58</v>
       </c>
       <c r="G88">
-        <v>1.4765577803218578E+80</v>
+        <v>-4.9476684598711092E+25</v>
       </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C89">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D89">
-        <v>3.1622776601683572E+40</v>
+        <v>1</v>
       </c>
       <c r="E89">
-        <v>3.4547476869599357E+20</v>
+        <v>1.6435284159071862E-34</v>
       </c>
       <c r="F89">
-        <v>-3.9846856799567184E+60</v>
+        <v>-3.5951993820309627E+59</v>
       </c>
       <c r="G89">
-        <v>-1.376608363609285E+81</v>
+        <v>-5.9088123452198432E+25</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C90">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D90">
-        <v>9.9999999999999285E+40</v>
+        <v>1</v>
       </c>
       <c r="E90">
-        <v>4.5376285572355542E+20</v>
+        <v>5.0084772659569421E-35</v>
       </c>
       <c r="F90">
-        <v>-4.6592448184899135E+61</v>
+        <v>7.8106463940249111E+60</v>
       </c>
       <c r="G90">
-        <v>-2.1141922343531618E+82</v>
+        <v>3.9119444896902334E+26</v>
       </c>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C91">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D91">
-        <v>3.1622776601683566E+41</v>
+        <v>1</v>
       </c>
       <c r="E91">
-        <v>5.9393446832697757E+20</v>
+        <v>1.5221779019837085E-35</v>
       </c>
       <c r="F91">
-        <v>3.2606966661791771E+62</v>
+        <v>2.166998853862898E+61</v>
       </c>
       <c r="G91">
-        <v>1.9366401408026777E+83</v>
+        <v>3.2985577689741272E+26</v>
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C92">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D92">
-        <v>9.9999999999999277E+41</v>
+        <v>1</v>
       </c>
       <c r="E92">
-        <v>7.7475843810841251E+20</v>
+        <v>4.6139426392097526E-36</v>
       </c>
       <c r="F92">
-        <v>3.9463726141933186E+63</v>
+        <v>-6.6995363924269665E+62</v>
       </c>
       <c r="G92">
-        <v>3.0574854827662282E+84</v>
+        <v>-3.0911276623956264E+27</v>
       </c>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C93">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D93">
-        <v>3.1622776601683564E+42</v>
+        <v>1</v>
       </c>
       <c r="E93">
-        <v>1.0072400096910994E+21</v>
+        <v>1.3948949398512401E-36</v>
       </c>
       <c r="F93">
-        <v>-2.7321284401103677E+64</v>
+        <v>-1.1503253980021377E+63</v>
       </c>
       <c r="G93">
-        <v>-2.7519090764940951E+85</v>
+        <v>-1.6045830768555456E+27</v>
       </c>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C94">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D94">
-        <v>9.9999999999999271E+42</v>
+        <v>1</v>
       </c>
       <c r="E94">
-        <v>1.3051446104021339E+21</v>
+        <v>4.2061853822878915E-37</v>
       </c>
       <c r="F94">
-        <v>-3.4212017326073579E+65</v>
+        <v>5.8096384733631357E+64</v>
       </c>
       <c r="G94">
-        <v>-4.4651630024109358E+86</v>
+        <v>2.4436416423037363E+28</v>
       </c>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C95">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D95">
-        <v>3.1622776601683561E+43</v>
+        <v>1</v>
       </c>
       <c r="E95">
-        <v>1.6856327028843023E+21</v>
+        <v>1.2651080739388634E-37</v>
       </c>
       <c r="F95">
-        <v>2.3427397255699465E+66</v>
+        <v>4.0831599494552486E+64</v>
       </c>
       <c r="G95">
-        <v>3.9489986957668976E+87</v>
+        <v>5.1656386192396365E+27</v>
       </c>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C96">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D96">
-        <v>9.9999999999999256E+43</v>
+        <v>1</v>
       </c>
       <c r="E96">
-        <v>2.1700266020873833E+21</v>
+        <v>3.7955393521133437E-38</v>
       </c>
       <c r="F96">
-        <v>3.0340849219501741E+67</v>
+        <v>-5.0952170713204804E+66</v>
       </c>
       <c r="G96">
-        <v>6.5840449936240996E+88</v>
+        <v>-1.9339096901756583E+29</v>
       </c>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C97">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D97">
-        <v>3.1622776601683557E+44</v>
+        <v>1</v>
       </c>
       <c r="E97">
-        <v>2.7847334907196122E+21</v>
+        <v>1.1358998064750436E-38</v>
       </c>
       <c r="F97">
-        <v>-2.0546975065377505E+68</v>
+        <v>1.5020363157998613E+66</v>
       </c>
       <c r="G97">
-        <v>-5.7217849597537531E+89</v>
+        <v>1.7061627604355498E+28</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C98">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D98">
-        <v>9.9999999999999248E+44</v>
+        <v>1</v>
       </c>
       <c r="E98">
-        <v>3.5623526450014532E+21</v>
+        <v>3.391102199261974E-39</v>
       </c>
       <c r="F98">
-        <v>-2.7512234048205342E+69</v>
+        <v>4.5197228303172288E+68</v>
       </c>
       <c r="G98">
-        <v>-9.8008279731523336E+90</v>
+        <v>1.5326842029943309E+30</v>
       </c>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C99">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D99">
-        <v>3.1622776601683554E+45</v>
+        <v>1</v>
       </c>
       <c r="E99">
-        <v>4.5429991184849484E+21</v>
+        <v>1.0099256595014657E-39</v>
       </c>
       <c r="F99">
-        <v>1.8422624969011475E+70</v>
+        <v>-5.8715555145371036E+68</v>
       </c>
       <c r="G99">
-        <v>8.3693968994397936E+91</v>
+        <v>-5.9298345753183524E+29</v>
       </c>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C100">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D100">
-        <v>9.9999999999999239E+45</v>
+        <v>1</v>
       </c>
       <c r="E100">
-        <v>5.7758808575420137E+21</v>
+        <v>3.0005346681953373E-40</v>
       </c>
       <c r="F100">
-        <v>2.5495481574039026E+71</v>
+        <v>-4.0542322204433073E+70</v>
       </c>
       <c r="G100">
-        <v>1.4725886397730714E+93</v>
+        <v>-1.2164864330354705E+31</v>
       </c>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C101">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D101">
-        <v>3.1622776601683544E+46</v>
+        <v>1</v>
       </c>
       <c r="E101">
-        <v>7.3211714674623408E+21</v>
+        <v>8.8936768469244698E-41</v>
       </c>
       <c r="F101">
-        <v>-1.6878086405440281E+72</v>
+        <v>9.4560632938174434E+70</v>
       </c>
       <c r="G101">
-        <v>-1.2356736461687341E+94</v>
+        <v>8.4099171179276535E+30</v>
       </c>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C102">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D102">
-        <v>9.9999999999999213E+46</v>
+        <v>1</v>
       </c>
       <c r="E102">
-        <v>9.252226639285824E+21</v>
+        <v>2.6299648581025865E-41</v>
       </c>
       <c r="F102">
-        <v>-2.4134533543651086E+73</v>
+        <v>3.6758753320741012E+72</v>
       </c>
       <c r="G102">
-        <v>-2.2329817417930589E+95</v>
+        <v>9.6674229461210609E+31</v>
       </c>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C103">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D103">
-        <v>3.1622776601683542E+47</v>
+        <v>1</v>
       </c>
       <c r="E103">
-        <v>1.1658198606457963E+22</v>
+        <v>7.7591941611810038E-42</v>
       </c>
       <c r="F103">
-        <v>1.5792836749731758E+74</v>
+        <v>-1.2564574828262499E+73</v>
       </c>
       <c r="G103">
-        <v>1.8411602738774087E+96</v>
+        <v>-9.7490975645176188E+31</v>
       </c>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C104">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D104">
-        <v>9.9999999999999193E+47</v>
+        <v>1</v>
       </c>
       <c r="E104">
-        <v>1.4647109943328451E+22</v>
+        <v>2.283985100848297E-42</v>
       </c>
       <c r="F104">
-        <v>2.3327080569402361E+75</v>
+        <v>-3.366435817187771E+74</v>
       </c>
       <c r="G104">
-        <v>3.4167431375691722E+97</v>
+        <v>-7.6888892494189303E+32</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C105">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D105">
-        <v>3.1622776601683533E+48</v>
+        <v>1</v>
       </c>
       <c r="E105">
-        <v>1.83494555533973E+22</v>
+        <v>6.7079763599362668E-43</v>
       </c>
       <c r="F105">
-        <v>-1.5085780841545783E+76</v>
+        <v>1.5428427652319768E+75</v>
       </c>
       <c r="G105">
-        <v>-2.7681586504023684E+98</v>
+        <v>1.03493527962748E+33</v>
       </c>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C106">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D106">
-        <v>9.9999999999999177E+48</v>
+        <v>1</v>
       </c>
       <c r="E106">
-        <v>2.2922409824241242E+22</v>
+        <v>1.9657250550619484E-43</v>
       </c>
       <c r="F106">
-        <v>-2.3011396766429772E+77</v>
+        <v>3.1111584661489404E+76</v>
       </c>
       <c r="G106">
-        <v>-5.2747666730832298E+99</v>
+        <v>6.1156821471770734E+33</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C107">
+        <v>1</v>
+      </c>
       <c r="D107">
-        <v>3.1622776601683523E+49</v>
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>5.747753747209044E-44</v>
+      </c>
+      <c r="F107">
+        <v>-1.8231017565422313E+77</v>
+      </c>
+      <c r="G107">
+        <v>-1.0478739952709E+34</v>
       </c>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.45">
       <c r="D108">
-        <v>9.9999999999999156E+49</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="D109">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
const some things fix operator* for shift
</commit_message>
<xml_diff>
--- a/gop.xlsx
+++ b/gop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\tmp\GR6250-2019\hw6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93B543F-2FD4-4342-8F12-A843907EF7F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E596120-B428-42FF-ACA5-0F53BFD0F51B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{D3B39B31-0FCC-485C-968B-EB7A4BAB9E1D}"/>
   </bookViews>
@@ -16,8 +16,13 @@
     <sheet name="Normal" sheetId="2" r:id="rId1"/>
     <sheet name="Poisson" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="f">Normal!$L$3</definedName>
+    <definedName name="k">Normal!$L$5</definedName>
+    <definedName name="sigma">Normal!$L$4</definedName>
+    <definedName name="t">Normal!$L$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -490,11 +495,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7A4851-E416-476B-A3BE-EC3AA0559FF7}">
-  <dimension ref="B2:L110"/>
+  <dimension ref="B2:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -504,13 +507,13 @@
     <col min="12" max="12" width="12.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.45">
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E2" cm="1">
         <f t="array" ref="E2">_xll.XLL.SEQUENCE.LIST({0,0})</f>
-        <v>-58650962</v>
+        <v>28247486</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
@@ -519,13 +522,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.45">
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E3" cm="1">
         <f t="array" ref="E3">_xll.XLL.SEQUENCE.CONCATENATE(E2,D7)</f>
-        <v>-58659264</v>
+        <v>29750150</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>6</v>
@@ -541,15 +544,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
       <c r="K4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +570,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B6" s="1"/>
       <c r="D6">
         <v>1</v>
@@ -592,16 +595,16 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7" cm="1">
         <f t="array" ref="C7">_xll.XLL.CUMULANT.NORMAL()</f>
-        <v>27669630</v>
+        <v>28156024</v>
       </c>
       <c r="D7">
-        <v>-23690</v>
+        <v>28155864</v>
       </c>
       <c r="G7">
         <f>MIN(_xll.XLL.SEQUENCE.TAKE(C9,G8))</f>
@@ -611,34 +614,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C8" cm="1">
         <f t="array" ref="C8">_xll.XLL.CUMULANT.SCALE(C7, C5)</f>
-        <v>27669810</v>
+        <v>28155664</v>
       </c>
       <c r="E8" cm="1">
         <f t="array" ref="E8">_xll.XLL.BELL.REDUCED(E3,1)</f>
-        <v>-58650998</v>
+        <v>28247090</v>
       </c>
       <c r="F8" cm="1">
         <f t="array" ref="F8">_xll.XLL.HERMITE(H3)</f>
-        <v>27986522</v>
+        <v>28593144</v>
       </c>
       <c r="G8" cm="1">
         <f t="array" ref="G8">_xll.XLL.SEQUENCE.MUL(E8,F8)</f>
-        <v>-58658802</v>
+        <v>29750136</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
@@ -657,11 +660,15 @@
         <v>2.2750131948179153E-2</v>
       </c>
       <c r="L9" cm="1">
-        <f t="array" ref="L9">_xll.XLL.OPTION.PUT(L3, L4*SQRT(L6), L5, C7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+        <f t="array" ref="L9">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I9, $C$7)</f>
+        <v>1.1335440964903825</v>
+      </c>
+      <c r="M9" cm="1">
+        <f t="array" ref="M9">_xll.XLL.BLACK.PUT.IMPLIED(f, L9, k + I9, t)</f>
+        <v>9.9999999999999756E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C10" s="5" cm="1">
         <f t="array" ref="C10:C19">_xll.XLL.SEQUENCE.TAKE(C9,C8)</f>
         <v>0</v>
@@ -690,8 +697,16 @@
         <f t="array" ref="K10">_xll.XLL.OPTION.CDF(I10, $C$8)</f>
         <v>2.8716559816001852E-2</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="L10" cm="1">
+        <f t="array" ref="L10">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I10, $C$7)</f>
+        <v>1.1691561797939087</v>
+      </c>
+      <c r="M10" cm="1">
+        <f t="array" ref="M10">_xll.XLL.BLACK.PUT.IMPLIED(f, L10, k + I10, t)</f>
+        <v>9.9999999999999797E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C11">
         <v>1</v>
       </c>
@@ -715,8 +730,16 @@
         <f t="array" ref="K11">_xll.XLL.OPTION.CDF(I11, $C$8)</f>
         <v>3.5930319112925768E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="L11" cm="1">
+        <f t="array" ref="L11">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I11, $C$7)</f>
+        <v>1.2055309119244129</v>
+      </c>
+      <c r="M11" cm="1">
+        <f t="array" ref="M11">_xll.XLL.BLACK.PUT.IMPLIED(f, L11, k + I11, t)</f>
+        <v>0.10000000000000019</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C12">
         <v>0</v>
       </c>
@@ -744,8 +767,16 @@
         <f t="array" ref="K12">_xll.XLL.OPTION.CDF(I12, $C$8)</f>
         <v>4.4565462758543062E-2</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="L12" cm="1">
+        <f t="array" ref="L12">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I12, $C$7)</f>
+        <v>1.2426729451030099</v>
+      </c>
+      <c r="M12" cm="1">
+        <f t="array" ref="M12">_xll.XLL.BLACK.PUT.IMPLIED(f, L12, k + I12, t)</f>
+        <v>9.9999999999999922E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C13">
         <v>0</v>
       </c>
@@ -772,8 +803,16 @@
         <f t="array" ref="K13">_xll.XLL.OPTION.CDF(I13, $C$8)</f>
         <v>5.4799291699557939E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="L13" cm="1">
+        <f t="array" ref="L13">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I13, $C$7)</f>
+        <v>1.2805866351889676</v>
+      </c>
+      <c r="M13" cm="1">
+        <f t="array" ref="M13">_xll.XLL.BLACK.PUT.IMPLIED(f, L13, k + I13, t)</f>
+        <v>0.10000000000000035</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C14">
         <v>0</v>
       </c>
@@ -800,8 +839,16 @@
         <f t="array" ref="K14">_xll.XLL.OPTION.CDF(I14, $C$8)</f>
         <v>6.6807201268858085E-2</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="L14" cm="1">
+        <f t="array" ref="L14">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I14, $C$7)</f>
+        <v>1.3192760373124983</v>
+      </c>
+      <c r="M14" cm="1">
+        <f t="array" ref="M14">_xll.XLL.BLACK.PUT.IMPLIED(f, L14, k + I14, t)</f>
+        <v>9.9999999999999589E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C15">
         <v>0</v>
       </c>
@@ -828,8 +875,16 @@
         <f t="array" ref="K15">_xll.XLL.OPTION.CDF(I15, $C$8)</f>
         <v>8.0756659233771122E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="L15" cm="1">
+        <f t="array" ref="L15">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I15, $C$7)</f>
+        <v>1.3587449018757169</v>
+      </c>
+      <c r="M15" cm="1">
+        <f t="array" ref="M15">_xll.XLL.BLACK.PUT.IMPLIED(f, L15, k + I15, t)</f>
+        <v>9.9999999999999756E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C16">
         <v>0</v>
       </c>
@@ -856,8 +911,16 @@
         <f t="array" ref="K16">_xll.XLL.OPTION.CDF(I16, $C$8)</f>
         <v>9.6800484585610358E-2</v>
       </c>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L16" cm="1">
+        <f t="array" ref="L16">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I16, $C$7)</f>
+        <v>1.3989966709276658</v>
+      </c>
+      <c r="M16" cm="1">
+        <f t="array" ref="M16">_xll.XLL.BLACK.PUT.IMPLIED(f, L16, k + I16, t)</f>
+        <v>0.10000000000001519</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.45">
       <c r="C17">
         <v>0</v>
       </c>
@@ -884,8 +947,16 @@
         <f t="array" ref="K17">_xll.XLL.OPTION.CDF(I17, $C$8)</f>
         <v>0.11506967022170833</v>
       </c>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L17" cm="1">
+        <f t="array" ref="L17">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I17, $C$7)</f>
+        <v>1.4400344749191731</v>
+      </c>
+      <c r="M17" cm="1">
+        <f t="array" ref="M17">_xll.XLL.BLACK.PUT.IMPLIED(f, L17, k + I17, t)</f>
+        <v>0.1000000000000045</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.45">
       <c r="C18">
         <v>0</v>
       </c>
@@ -912,8 +983,16 @@
         <f t="array" ref="K18">_xll.XLL.OPTION.CDF(I18, $C$8)</f>
         <v>0.13566606094638267</v>
       </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L18" cm="1">
+        <f t="array" ref="L18">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I18, $C$7)</f>
+        <v>1.4818611298421018</v>
+      </c>
+      <c r="M18" cm="1">
+        <f t="array" ref="M18">_xll.XLL.BLACK.PUT.IMPLIED(f, L18, k + I18, t)</f>
+        <v>0.10000000000000184</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.45">
       <c r="C19">
         <v>0</v>
       </c>
@@ -940,8 +1019,16 @@
         <f t="array" ref="K19">_xll.XLL.OPTION.CDF(I19, $C$8)</f>
         <v>0.15865525393145713</v>
       </c>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L19" cm="1">
+        <f t="array" ref="L19">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I19, $C$7)</f>
+        <v>1.5244791347568096</v>
+      </c>
+      <c r="M19" cm="1">
+        <f t="array" ref="M19">_xll.XLL.BLACK.PUT.IMPLIED(f, L19, k + I19, t)</f>
+        <v>0.1000000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.45">
       <c r="D20">
         <v>0</v>
       </c>
@@ -956,8 +1043,16 @@
         <f t="array" ref="K20">_xll.XLL.OPTION.CDF(I20, $C$8)</f>
         <v>0.18406012534675947</v>
       </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L20" cm="1">
+        <f t="array" ref="L20">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I20, $C$7)</f>
+        <v>1.5678906697111401</v>
+      </c>
+      <c r="M20" cm="1">
+        <f t="array" ref="M20">_xll.XLL.BLACK.PUT.IMPLIED(f, L20, k + I20, t)</f>
+        <v>9.9999999999999936E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.45">
       <c r="D21">
         <v>0</v>
       </c>
@@ -972,8 +1067,16 @@
         <f t="array" ref="K21">_xll.XLL.OPTION.CDF(I21, $C$8)</f>
         <v>0.21185539858339675</v>
       </c>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L21" cm="1">
+        <f t="array" ref="L21">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I21, $C$7)</f>
+        <v>1.6120975940529334</v>
+      </c>
+      <c r="M21" cm="1">
+        <f t="array" ref="M21">_xll.XLL.BLACK.PUT.IMPLIED(f, L21, k + I21, t)</f>
+        <v>9.9999999999999811E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I22">
         <v>-0.7</v>
       </c>
@@ -985,8 +1088,16 @@
         <f t="array" ref="K22">_xll.XLL.OPTION.CDF(I22, $C$8)</f>
         <v>0.24196365222307309</v>
       </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L22" cm="1">
+        <f t="array" ref="L22">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I22, $C$7)</f>
+        <v>1.6571014451376413</v>
+      </c>
+      <c r="M22" cm="1">
+        <f t="array" ref="M22">_xll.XLL.BLACK.PUT.IMPLIED(f, L22, k + I22, t)</f>
+        <v>9.9999999999999867E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I23">
         <v>-0.6</v>
       </c>
@@ -998,8 +1109,16 @@
         <f t="array" ref="K23">_xll.XLL.OPTION.CDF(I23, $C$8)</f>
         <v>0.27425311775007361</v>
       </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L23" cm="1">
+        <f t="array" ref="L23">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I23, $C$7)</f>
+        <v>1.7029034374317291</v>
+      </c>
+      <c r="M23" cm="1">
+        <f t="array" ref="M23">_xll.XLL.BLACK.PUT.IMPLIED(f, L23, k + I23, t)</f>
+        <v>9.999999999999977E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I24">
         <v>-0.5</v>
       </c>
@@ -1011,8 +1130,16 @@
         <f t="array" ref="K24">_xll.XLL.OPTION.CDF(I24, $C$8)</f>
         <v>0.30853753872598694</v>
       </c>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L24" cm="1">
+        <f t="array" ref="L24">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I24, $C$7)</f>
+        <v>1.7495044620115578</v>
+      </c>
+      <c r="M24" cm="1">
+        <f t="array" ref="M24">_xll.XLL.BLACK.PUT.IMPLIED(f, L24, k + I24, t)</f>
+        <v>9.9999999999999353E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I25">
         <v>-0.4</v>
       </c>
@@ -1024,8 +1151,16 @@
         <f t="array" ref="K25">_xll.XLL.OPTION.CDF(I25, $C$8)</f>
         <v>0.34457825838967582</v>
       </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L25" cm="1">
+        <f t="array" ref="L25">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I25, $C$7)</f>
+        <v>1.796905086456988</v>
+      </c>
+      <c r="M25" cm="1">
+        <f t="array" ref="M25">_xll.XLL.BLACK.PUT.IMPLIED(f, L25, k + I25, t)</f>
+        <v>0.10000000000000012</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I26">
         <v>-0.3</v>
       </c>
@@ -1037,8 +1172,16 @@
         <f t="array" ref="K26">_xll.XLL.OPTION.CDF(I26, $C$8)</f>
         <v>0.38208857781104738</v>
       </c>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L26" cm="1">
+        <f t="array" ref="L26">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I26, $C$7)</f>
+        <v>1.8451055551376427</v>
+      </c>
+      <c r="M26" cm="1">
+        <f t="array" ref="M26">_xll.XLL.BLACK.PUT.IMPLIED(f, L26, k + I26, t)</f>
+        <v>0.10000000000000062</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I27">
         <v>-0.2</v>
       </c>
@@ -1050,8 +1193,16 @@
         <f t="array" ref="K27">_xll.XLL.OPTION.CDF(I27, $C$8)</f>
         <v>0.42074029056089696</v>
       </c>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L27" cm="1">
+        <f t="array" ref="L27">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I27, $C$7)</f>
+        <v>1.8941057898895295</v>
+      </c>
+      <c r="M27" cm="1">
+        <f t="array" ref="M27">_xll.XLL.BLACK.PUT.IMPLIED(f, L27, k + I27, t)</f>
+        <v>0.10000000000000064</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I28">
         <v>-0.1</v>
       </c>
@@ -1063,8 +1214,16 @@
         <f t="array" ref="K28">_xll.XLL.OPTION.CDF(I28, $C$8)</f>
         <v>0.46017216272297101</v>
       </c>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L28" cm="1">
+        <f t="array" ref="L28">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I28, $C$7)</f>
+        <v>1.9439053910786939</v>
+      </c>
+      <c r="M28" cm="1">
+        <f t="array" ref="M28">_xll.XLL.BLACK.PUT.IMPLIED(f, L28, k + I28, t)</f>
+        <v>0.10000000000000049</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I29">
         <v>0</v>
       </c>
@@ -1076,8 +1235,16 @@
         <f t="array" ref="K29">_xll.XLL.OPTION.CDF(I29, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L29" cm="1">
+        <f t="array" ref="L29">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I29, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M29" cm="1">
+        <f t="array" ref="M29">_xll.XLL.BLACK.PUT.IMPLIED(f, L29, k + I29, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I30">
         <v>0.1</v>
       </c>
@@ -1089,8 +1256,16 @@
         <f t="array" ref="K30">_xll.XLL.OPTION.CDF(I30, $C$8)</f>
         <v>0.53982783727702899</v>
       </c>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L30" cm="1">
+        <f t="array" ref="L30">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I30, $C$7)</f>
+        <v>2.0458994959397998</v>
+      </c>
+      <c r="M30" cm="1">
+        <f t="array" ref="M30">_xll.XLL.BLACK.PUT.IMPLIED(f, L30, k + I30, t)</f>
+        <v>0.10000000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I31">
         <v>0.2</v>
       </c>
@@ -1102,8 +1277,16 @@
         <f t="array" ref="K31">_xll.XLL.OPTION.CDF(I31, $C$8)</f>
         <v>0.57925970943910299</v>
       </c>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="L31" cm="1">
+        <f t="array" ref="L31">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I31, $C$7)</f>
+        <v>2.098091607896869</v>
+      </c>
+      <c r="M31" cm="1">
+        <f t="array" ref="M31">_xll.XLL.BLACK.PUT.IMPLIED(f, L31, k + I31, t)</f>
+        <v>0.10000000000000027</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I32">
         <v>0.3</v>
       </c>
@@ -1115,8 +1298,16 @@
         <f t="array" ref="K32">_xll.XLL.OPTION.CDF(I32, $C$8)</f>
         <v>0.61791142218895256</v>
       </c>
-    </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L32" cm="1">
+        <f t="array" ref="L32">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I32, $C$7)</f>
+        <v>2.1510783076219155</v>
+      </c>
+      <c r="M32" cm="1">
+        <f t="array" ref="M32">_xll.XLL.BLACK.PUT.IMPLIED(f, L32, k + I32, t)</f>
+        <v>9.9999999999999561E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I33">
         <v>0.4</v>
       </c>
@@ -1128,8 +1319,16 @@
         <f t="array" ref="K33">_xll.XLL.OPTION.CDF(I33, $C$8)</f>
         <v>0.65542174161032418</v>
       </c>
-    </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L33" cm="1">
+        <f t="array" ref="L33">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I33, $C$7)</f>
+        <v>2.2048576173023449</v>
+      </c>
+      <c r="M33" cm="1">
+        <f t="array" ref="M33">_xll.XLL.BLACK.PUT.IMPLIED(f, L33, k + I33, t)</f>
+        <v>0.10000000000000031</v>
+      </c>
+    </row>
+    <row r="34" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I34">
         <v>0.5</v>
       </c>
@@ -1141,8 +1340,16 @@
         <f t="array" ref="K34">_xll.XLL.OPTION.CDF(I34, $C$8)</f>
         <v>0.69146246127401301</v>
       </c>
-    </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L34" cm="1">
+        <f t="array" ref="L34">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I34, $C$7)</f>
+        <v>2.2594272518844889</v>
+      </c>
+      <c r="M34" cm="1">
+        <f t="array" ref="M34">_xll.XLL.BLACK.PUT.IMPLIED(f, L34, k + I34, t)</f>
+        <v>9.9999999999999645E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I35">
         <v>0.6</v>
       </c>
@@ -1154,8 +1361,16 @@
         <f t="array" ref="K35">_xll.XLL.OPTION.CDF(I35, $C$8)</f>
         <v>0.72574688224992645</v>
       </c>
-    </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L35" cm="1">
+        <f t="array" ref="L35">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I35, $C$7)</f>
+        <v>2.3147846226919455</v>
+      </c>
+      <c r="M35" cm="1">
+        <f t="array" ref="M35">_xll.XLL.BLACK.PUT.IMPLIED(f, L35, k + I35, t)</f>
+        <v>0.10000000000000024</v>
+      </c>
+    </row>
+    <row r="36" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I36">
         <v>0.7</v>
       </c>
@@ -1167,8 +1382,16 @@
         <f t="array" ref="K36">_xll.XLL.OPTION.CDF(I36, $C$8)</f>
         <v>0.75803634777692697</v>
       </c>
-    </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L36" cm="1">
+        <f t="array" ref="L36">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I36, $C$7)</f>
+        <v>2.3709268413786333</v>
+      </c>
+      <c r="M36" cm="1">
+        <f t="array" ref="M36">_xll.XLL.BLACK.PUT.IMPLIED(f, L36, k + I36, t)</f>
+        <v>9.9999999999999895E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I37">
         <v>0.8</v>
       </c>
@@ -1180,8 +1403,16 @@
         <f t="array" ref="K37">_xll.XLL.OPTION.CDF(I37, $C$8)</f>
         <v>0.78814460141660325</v>
       </c>
-    </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L37" cm="1">
+        <f t="array" ref="L37">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I37, $C$7)</f>
+        <v>2.4278507242075094</v>
+      </c>
+      <c r="M37" cm="1">
+        <f t="array" ref="M37">_xll.XLL.BLACK.PUT.IMPLIED(f, L37, k + I37, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I38">
         <v>0.9</v>
       </c>
@@ -1193,8 +1424,16 @@
         <f t="array" ref="K38">_xll.XLL.OPTION.CDF(I38, $C$8)</f>
         <v>0.81593987465324047</v>
       </c>
-    </row>
-    <row r="39" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L38" cm="1">
+        <f t="array" ref="L38">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I38, $C$7)</f>
+        <v>2.4855527966447042</v>
+      </c>
+      <c r="M38" cm="1">
+        <f t="array" ref="M38">_xll.XLL.BLACK.PUT.IMPLIED(f, L38, k + I38, t)</f>
+        <v>0.10000000000000071</v>
+      </c>
+    </row>
+    <row r="39" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I39">
         <v>1</v>
       </c>
@@ -1206,8 +1445,16 @@
         <f t="array" ref="K39">_xll.XLL.OPTION.CDF(I39, $C$8)</f>
         <v>0.84134474606854281</v>
       </c>
-    </row>
-    <row r="40" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L39" cm="1">
+        <f t="array" ref="L39">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I39, $C$7)</f>
+        <v>2.5440292982588346</v>
+      </c>
+      <c r="M39" cm="1">
+        <f t="array" ref="M39">_xll.XLL.BLACK.PUT.IMPLIED(f, L39, k + I39, t)</f>
+        <v>0.1000000000000006</v>
+      </c>
+    </row>
+    <row r="40" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I40">
         <v>1.1000000000000001</v>
       </c>
@@ -1219,8 +1466,16 @@
         <f t="array" ref="K40">_xll.XLL.OPTION.CDF(I40, $C$8)</f>
         <v>0.86433393905361733</v>
       </c>
-    </row>
-    <row r="41" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L40" cm="1">
+        <f t="array" ref="L40">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I40, $C$7)</f>
+        <v>2.6032761879147515</v>
+      </c>
+      <c r="M40" cm="1">
+        <f t="array" ref="M40">_xll.XLL.BLACK.PUT.IMPLIED(f, L40, k + I40, t)</f>
+        <v>0.10000000000000096</v>
+      </c>
+    </row>
+    <row r="41" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I41">
         <v>1.2</v>
       </c>
@@ -1232,8 +1487,16 @@
         <f t="array" ref="K41">_xll.XLL.OPTION.CDF(I41, $C$8)</f>
         <v>0.88493032977829167</v>
       </c>
-    </row>
-    <row r="42" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L41" cm="1">
+        <f t="array" ref="L41">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I41, $C$7)</f>
+        <v>2.6632891492498629</v>
+      </c>
+      <c r="M41" cm="1">
+        <f t="array" ref="M41">_xll.XLL.BLACK.PUT.IMPLIED(f, L41, k + I41, t)</f>
+        <v>0.10000000000000477</v>
+      </c>
+    </row>
+    <row r="42" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I42">
         <v>1.3</v>
       </c>
@@ -1245,8 +1508,16 @@
         <f t="array" ref="K42">_xll.XLL.OPTION.CDF(I42, $C$8)</f>
         <v>0.9031995154143897</v>
       </c>
-    </row>
-    <row r="43" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L42" cm="1">
+        <f t="array" ref="L42">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I42, $C$7)</f>
+        <v>2.7240635964217077</v>
+      </c>
+      <c r="M42" cm="1">
+        <f t="array" ref="M42">_xll.XLL.BLACK.PUT.IMPLIED(f, L42, k + I42, t)</f>
+        <v>0.10000000000001216</v>
+      </c>
+    </row>
+    <row r="43" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I43">
         <v>1.4</v>
       </c>
@@ -1258,8 +1529,16 @@
         <f t="array" ref="K43">_xll.XLL.OPTION.CDF(I43, $C$8)</f>
         <v>0.91924334076622882</v>
       </c>
-    </row>
-    <row r="44" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L43" cm="1">
+        <f t="array" ref="L43">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I43, $C$7)</f>
+        <v>2.7855946801146558</v>
+      </c>
+      <c r="M43" cm="1">
+        <f t="array" ref="M43">_xll.XLL.BLACK.PUT.IMPLIED(f, L43, k + I43, t)</f>
+        <v>0.10000000000000045</v>
+      </c>
+    </row>
+    <row r="44" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I44">
         <v>1.5</v>
       </c>
@@ -1271,8 +1550,16 @@
         <f t="array" ref="K44">_xll.XLL.OPTION.CDF(I44, $C$8)</f>
         <v>0.93319279873114191</v>
       </c>
-    </row>
-    <row r="45" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L44" cm="1">
+        <f t="array" ref="L44">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I44, $C$7)</f>
+        <v>2.8478772937926635</v>
+      </c>
+      <c r="M44" cm="1">
+        <f t="array" ref="M44">_xll.XLL.BLACK.PUT.IMPLIED(f, L44, k + I44, t)</f>
+        <v>0.10000000000000024</v>
+      </c>
+    </row>
+    <row r="45" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I45">
         <v>1.6</v>
       </c>
@@ -1284,8 +1571,16 @@
         <f t="array" ref="K45">_xll.XLL.OPTION.CDF(I45, $C$8)</f>
         <v>0.94520070830044212</v>
       </c>
-    </row>
-    <row r="46" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L45" cm="1">
+        <f t="array" ref="L45">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I45, $C$7)</f>
+        <v>2.9109060801860522</v>
+      </c>
+      <c r="M45" cm="1">
+        <f t="array" ref="M45">_xll.XLL.BLACK.PUT.IMPLIED(f, L45, k + I45, t)</f>
+        <v>0.1000000000000006</v>
+      </c>
+    </row>
+    <row r="46" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I46">
         <v>1.7</v>
       </c>
@@ -1297,8 +1592,16 @@
         <f t="array" ref="K46">_xll.XLL.OPTION.CDF(I46, $C$8)</f>
         <v>0.95543453724145699</v>
       </c>
-    </row>
-    <row r="47" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L46" cm="1">
+        <f t="array" ref="L46">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I46, $C$7)</f>
+        <v>2.974675437998485</v>
+      </c>
+      <c r="M46" cm="1">
+        <f t="array" ref="M46">_xll.XLL.BLACK.PUT.IMPLIED(f, L46, k + I46, t)</f>
+        <v>9.9999999999999631E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I47">
         <v>1.8</v>
       </c>
@@ -1310,8 +1613,16 @@
         <f t="array" ref="K47">_xll.XLL.OPTION.CDF(I47, $C$8)</f>
         <v>0.96406968088707423</v>
       </c>
-    </row>
-    <row r="48" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L47" cm="1">
+        <f t="array" ref="L47">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I47, $C$7)</f>
+        <v>3.0391795288213501</v>
+      </c>
+      <c r="M47" cm="1">
+        <f t="array" ref="M47">_xll.XLL.BLACK.PUT.IMPLIED(f, L47, k + I47, t)</f>
+        <v>9.9999999999999228E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I48">
         <v>1.9</v>
       </c>
@@ -1323,8 +1634,16 @@
         <f t="array" ref="K48">_xll.XLL.OPTION.CDF(I48, $C$8)</f>
         <v>0.97128344018399815</v>
       </c>
-    </row>
-    <row r="49" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L48" cm="1">
+        <f t="array" ref="L48">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I48, $C$7)</f>
+        <v>3.1044122842416968</v>
+      </c>
+      <c r="M48" cm="1">
+        <f t="array" ref="M48">_xll.XLL.BLACK.PUT.IMPLIED(f, L48, k + I48, t)</f>
+        <v>0.10000000000000024</v>
+      </c>
+    </row>
+    <row r="49" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I49">
         <v>2</v>
       </c>
@@ -1336,8 +1655,16 @@
         <f t="array" ref="K49">_xll.XLL.OPTION.CDF(I49, $C$8)</f>
         <v>0.9772498680518209</v>
       </c>
-    </row>
-    <row r="50" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L49" cm="1">
+        <f t="array" ref="L49">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I49, $C$7)</f>
+        <v>3.1703674131298101</v>
+      </c>
+      <c r="M49" cm="1">
+        <f t="array" ref="M49">_xll.XLL.BLACK.PUT.IMPLIED(f, L49, k + I49, t)</f>
+        <v>0.10000000000000034</v>
+      </c>
+    </row>
+    <row r="50" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J50" cm="1">
         <f t="array" ref="J50">_xll.XLL.OPTION.PDF(I50, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1346,8 +1673,16 @@
         <f t="array" ref="K50">_xll.XLL.OPTION.CDF(I50, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="51" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L50" cm="1">
+        <f t="array" ref="L50">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I50, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M50" cm="1">
+        <f t="array" ref="M50">_xll.XLL.BLACK.PUT.IMPLIED(f, L50, k + I50, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J51" cm="1">
         <f t="array" ref="J51">_xll.XLL.OPTION.PDF(I51, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1356,8 +1691,16 @@
         <f t="array" ref="K51">_xll.XLL.OPTION.CDF(I51, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="52" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L51" cm="1">
+        <f t="array" ref="L51">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I51, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M51" cm="1">
+        <f t="array" ref="M51">_xll.XLL.BLACK.PUT.IMPLIED(f, L51, k + I51, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J52" cm="1">
         <f t="array" ref="J52">_xll.XLL.OPTION.PDF(I52, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1366,8 +1709,16 @@
         <f t="array" ref="K52">_xll.XLL.OPTION.CDF(I52, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="53" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L52" cm="1">
+        <f t="array" ref="L52">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I52, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M52" cm="1">
+        <f t="array" ref="M52">_xll.XLL.BLACK.PUT.IMPLIED(f, L52, k + I52, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J53" cm="1">
         <f t="array" ref="J53">_xll.XLL.OPTION.PDF(I53, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1376,8 +1727,16 @@
         <f t="array" ref="K53">_xll.XLL.OPTION.CDF(I53, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="54" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L53" cm="1">
+        <f t="array" ref="L53">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I53, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M53" cm="1">
+        <f t="array" ref="M53">_xll.XLL.BLACK.PUT.IMPLIED(f, L53, k + I53, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J54" cm="1">
         <f t="array" ref="J54">_xll.XLL.OPTION.PDF(I54, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1386,8 +1745,16 @@
         <f t="array" ref="K54">_xll.XLL.OPTION.CDF(I54, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="55" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L54" cm="1">
+        <f t="array" ref="L54">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I54, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M54" cm="1">
+        <f t="array" ref="M54">_xll.XLL.BLACK.PUT.IMPLIED(f, L54, k + I54, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J55" cm="1">
         <f t="array" ref="J55">_xll.XLL.OPTION.PDF(I55, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1396,8 +1763,16 @@
         <f t="array" ref="K55">_xll.XLL.OPTION.CDF(I55, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="56" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L55" cm="1">
+        <f t="array" ref="L55">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I55, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M55" cm="1">
+        <f t="array" ref="M55">_xll.XLL.BLACK.PUT.IMPLIED(f, L55, k + I55, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J56" cm="1">
         <f t="array" ref="J56">_xll.XLL.OPTION.PDF(I56, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1406,8 +1781,16 @@
         <f t="array" ref="K56">_xll.XLL.OPTION.CDF(I56, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="57" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L56" cm="1">
+        <f t="array" ref="L56">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I56, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M56" cm="1">
+        <f t="array" ref="M56">_xll.XLL.BLACK.PUT.IMPLIED(f, L56, k + I56, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J57" cm="1">
         <f t="array" ref="J57">_xll.XLL.OPTION.PDF(I57, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1416,8 +1799,16 @@
         <f t="array" ref="K57">_xll.XLL.OPTION.CDF(I57, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="58" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L57" cm="1">
+        <f t="array" ref="L57">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I57, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M57" cm="1">
+        <f t="array" ref="M57">_xll.XLL.BLACK.PUT.IMPLIED(f, L57, k + I57, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J58" cm="1">
         <f t="array" ref="J58">_xll.XLL.OPTION.PDF(I58, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1426,8 +1817,16 @@
         <f t="array" ref="K58">_xll.XLL.OPTION.CDF(I58, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="59" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L58" cm="1">
+        <f t="array" ref="L58">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I58, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M58" cm="1">
+        <f t="array" ref="M58">_xll.XLL.BLACK.PUT.IMPLIED(f, L58, k + I58, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J59" cm="1">
         <f t="array" ref="J59">_xll.XLL.OPTION.PDF(I59, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1436,8 +1835,16 @@
         <f t="array" ref="K59">_xll.XLL.OPTION.CDF(I59, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="60" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L59" cm="1">
+        <f t="array" ref="L59">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I59, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M59" cm="1">
+        <f t="array" ref="M59">_xll.XLL.BLACK.PUT.IMPLIED(f, L59, k + I59, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J60" cm="1">
         <f t="array" ref="J60">_xll.XLL.OPTION.PDF(I60, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1446,8 +1853,16 @@
         <f t="array" ref="K60">_xll.XLL.OPTION.CDF(I60, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="61" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L60" cm="1">
+        <f t="array" ref="L60">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I60, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M60" cm="1">
+        <f t="array" ref="M60">_xll.XLL.BLACK.PUT.IMPLIED(f, L60, k + I60, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J61" cm="1">
         <f t="array" ref="J61">_xll.XLL.OPTION.PDF(I61, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1456,8 +1871,16 @@
         <f t="array" ref="K61">_xll.XLL.OPTION.CDF(I61, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="62" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L61" cm="1">
+        <f t="array" ref="L61">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I61, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M61" cm="1">
+        <f t="array" ref="M61">_xll.XLL.BLACK.PUT.IMPLIED(f, L61, k + I61, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J62" cm="1">
         <f t="array" ref="J62">_xll.XLL.OPTION.PDF(I62, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1466,8 +1889,16 @@
         <f t="array" ref="K62">_xll.XLL.OPTION.CDF(I62, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="63" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L62" cm="1">
+        <f t="array" ref="L62">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I62, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M62" cm="1">
+        <f t="array" ref="M62">_xll.XLL.BLACK.PUT.IMPLIED(f, L62, k + I62, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J63" cm="1">
         <f t="array" ref="J63">_xll.XLL.OPTION.PDF(I63, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1476,8 +1907,16 @@
         <f t="array" ref="K63">_xll.XLL.OPTION.CDF(I63, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="64" spans="9:11" x14ac:dyDescent="0.45">
+      <c r="L63" cm="1">
+        <f t="array" ref="L63">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I63, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M63" cm="1">
+        <f t="array" ref="M63">_xll.XLL.BLACK.PUT.IMPLIED(f, L63, k + I63, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="9:13" x14ac:dyDescent="0.45">
       <c r="J64" cm="1">
         <f t="array" ref="J64">_xll.XLL.OPTION.PDF(I64, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1486,8 +1925,16 @@
         <f t="array" ref="K64">_xll.XLL.OPTION.CDF(I64, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="65" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L64" cm="1">
+        <f t="array" ref="L64">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I64, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M64" cm="1">
+        <f t="array" ref="M64">_xll.XLL.BLACK.PUT.IMPLIED(f, L64, k + I64, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J65" cm="1">
         <f t="array" ref="J65">_xll.XLL.OPTION.PDF(I65, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1496,8 +1943,16 @@
         <f t="array" ref="K65">_xll.XLL.OPTION.CDF(I65, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="66" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L65" cm="1">
+        <f t="array" ref="L65">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I65, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M65" cm="1">
+        <f t="array" ref="M65">_xll.XLL.BLACK.PUT.IMPLIED(f, L65, k + I65, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J66" cm="1">
         <f t="array" ref="J66">_xll.XLL.OPTION.PDF(I66, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1506,8 +1961,16 @@
         <f t="array" ref="K66">_xll.XLL.OPTION.CDF(I66, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="67" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L66" cm="1">
+        <f t="array" ref="L66">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I66, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M66" cm="1">
+        <f t="array" ref="M66">_xll.XLL.BLACK.PUT.IMPLIED(f, L66, k + I66, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J67" cm="1">
         <f t="array" ref="J67">_xll.XLL.OPTION.PDF(I67, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1516,8 +1979,16 @@
         <f t="array" ref="K67">_xll.XLL.OPTION.CDF(I67, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="68" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L67" cm="1">
+        <f t="array" ref="L67">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I67, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M67" cm="1">
+        <f t="array" ref="M67">_xll.XLL.BLACK.PUT.IMPLIED(f, L67, k + I67, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J68" cm="1">
         <f t="array" ref="J68">_xll.XLL.OPTION.PDF(I68, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1526,8 +1997,16 @@
         <f t="array" ref="K68">_xll.XLL.OPTION.CDF(I68, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="69" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L68" cm="1">
+        <f t="array" ref="L68">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I68, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M68" cm="1">
+        <f t="array" ref="M68">_xll.XLL.BLACK.PUT.IMPLIED(f, L68, k + I68, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J69" cm="1">
         <f t="array" ref="J69">_xll.XLL.OPTION.PDF(I69, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1536,8 +2015,16 @@
         <f t="array" ref="K69">_xll.XLL.OPTION.CDF(I69, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="70" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L69" cm="1">
+        <f t="array" ref="L69">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I69, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M69" cm="1">
+        <f t="array" ref="M69">_xll.XLL.BLACK.PUT.IMPLIED(f, L69, k + I69, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J70" cm="1">
         <f t="array" ref="J70">_xll.XLL.OPTION.PDF(I70, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1546,8 +2033,16 @@
         <f t="array" ref="K70">_xll.XLL.OPTION.CDF(I70, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="71" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L70" cm="1">
+        <f t="array" ref="L70">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I70, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M70" cm="1">
+        <f t="array" ref="M70">_xll.XLL.BLACK.PUT.IMPLIED(f, L70, k + I70, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J71" cm="1">
         <f t="array" ref="J71">_xll.XLL.OPTION.PDF(I71, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1556,8 +2051,16 @@
         <f t="array" ref="K71">_xll.XLL.OPTION.CDF(I71, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="72" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L71" cm="1">
+        <f t="array" ref="L71">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I71, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M71" cm="1">
+        <f t="array" ref="M71">_xll.XLL.BLACK.PUT.IMPLIED(f, L71, k + I71, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J72" cm="1">
         <f t="array" ref="J72">_xll.XLL.OPTION.PDF(I72, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1566,8 +2069,16 @@
         <f t="array" ref="K72">_xll.XLL.OPTION.CDF(I72, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="73" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L72" cm="1">
+        <f t="array" ref="L72">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I72, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M72" cm="1">
+        <f t="array" ref="M72">_xll.XLL.BLACK.PUT.IMPLIED(f, L72, k + I72, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J73" cm="1">
         <f t="array" ref="J73">_xll.XLL.OPTION.PDF(I73, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1576,8 +2087,16 @@
         <f t="array" ref="K73">_xll.XLL.OPTION.CDF(I73, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="74" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L73" cm="1">
+        <f t="array" ref="L73">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I73, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M73" cm="1">
+        <f t="array" ref="M73">_xll.XLL.BLACK.PUT.IMPLIED(f, L73, k + I73, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J74" cm="1">
         <f t="array" ref="J74">_xll.XLL.OPTION.PDF(I74, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1586,8 +2105,16 @@
         <f t="array" ref="K74">_xll.XLL.OPTION.CDF(I74, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="75" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L74" cm="1">
+        <f t="array" ref="L74">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I74, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M74" cm="1">
+        <f t="array" ref="M74">_xll.XLL.BLACK.PUT.IMPLIED(f, L74, k + I74, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J75" cm="1">
         <f t="array" ref="J75">_xll.XLL.OPTION.PDF(I75, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1596,8 +2123,16 @@
         <f t="array" ref="K75">_xll.XLL.OPTION.CDF(I75, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="76" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L75" cm="1">
+        <f t="array" ref="L75">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I75, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M75" cm="1">
+        <f t="array" ref="M75">_xll.XLL.BLACK.PUT.IMPLIED(f, L75, k + I75, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J76" cm="1">
         <f t="array" ref="J76">_xll.XLL.OPTION.PDF(I76, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1606,8 +2141,16 @@
         <f t="array" ref="K76">_xll.XLL.OPTION.CDF(I76, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="77" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L76" cm="1">
+        <f t="array" ref="L76">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I76, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M76" cm="1">
+        <f t="array" ref="M76">_xll.XLL.BLACK.PUT.IMPLIED(f, L76, k + I76, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J77" cm="1">
         <f t="array" ref="J77">_xll.XLL.OPTION.PDF(I77, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1616,8 +2159,16 @@
         <f t="array" ref="K77">_xll.XLL.OPTION.CDF(I77, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="78" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L77" cm="1">
+        <f t="array" ref="L77">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I77, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M77" cm="1">
+        <f t="array" ref="M77">_xll.XLL.BLACK.PUT.IMPLIED(f, L77, k + I77, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J78" cm="1">
         <f t="array" ref="J78">_xll.XLL.OPTION.PDF(I78, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1626,8 +2177,16 @@
         <f t="array" ref="K78">_xll.XLL.OPTION.CDF(I78, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="79" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L78" cm="1">
+        <f t="array" ref="L78">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I78, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M78" cm="1">
+        <f t="array" ref="M78">_xll.XLL.BLACK.PUT.IMPLIED(f, L78, k + I78, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J79" cm="1">
         <f t="array" ref="J79">_xll.XLL.OPTION.PDF(I79, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1636,8 +2195,16 @@
         <f t="array" ref="K79">_xll.XLL.OPTION.CDF(I79, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="80" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L79" cm="1">
+        <f t="array" ref="L79">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I79, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M79" cm="1">
+        <f t="array" ref="M79">_xll.XLL.BLACK.PUT.IMPLIED(f, L79, k + I79, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J80" cm="1">
         <f t="array" ref="J80">_xll.XLL.OPTION.PDF(I80, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1646,8 +2213,16 @@
         <f t="array" ref="K80">_xll.XLL.OPTION.CDF(I80, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="81" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L80" cm="1">
+        <f t="array" ref="L80">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I80, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M80" cm="1">
+        <f t="array" ref="M80">_xll.XLL.BLACK.PUT.IMPLIED(f, L80, k + I80, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J81" cm="1">
         <f t="array" ref="J81">_xll.XLL.OPTION.PDF(I81, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1656,8 +2231,16 @@
         <f t="array" ref="K81">_xll.XLL.OPTION.CDF(I81, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="82" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L81" cm="1">
+        <f t="array" ref="L81">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I81, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M81" cm="1">
+        <f t="array" ref="M81">_xll.XLL.BLACK.PUT.IMPLIED(f, L81, k + I81, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J82" cm="1">
         <f t="array" ref="J82">_xll.XLL.OPTION.PDF(I82, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1666,8 +2249,16 @@
         <f t="array" ref="K82">_xll.XLL.OPTION.CDF(I82, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="83" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L82" cm="1">
+        <f t="array" ref="L82">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I82, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M82" cm="1">
+        <f t="array" ref="M82">_xll.XLL.BLACK.PUT.IMPLIED(f, L82, k + I82, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J83" cm="1">
         <f t="array" ref="J83">_xll.XLL.OPTION.PDF(I83, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1676,8 +2267,16 @@
         <f t="array" ref="K83">_xll.XLL.OPTION.CDF(I83, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="84" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L83" cm="1">
+        <f t="array" ref="L83">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I83, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M83" cm="1">
+        <f t="array" ref="M83">_xll.XLL.BLACK.PUT.IMPLIED(f, L83, k + I83, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J84" cm="1">
         <f t="array" ref="J84">_xll.XLL.OPTION.PDF(I84, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1686,8 +2285,16 @@
         <f t="array" ref="K84">_xll.XLL.OPTION.CDF(I84, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="85" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L84" cm="1">
+        <f t="array" ref="L84">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I84, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M84" cm="1">
+        <f t="array" ref="M84">_xll.XLL.BLACK.PUT.IMPLIED(f, L84, k + I84, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J85" cm="1">
         <f t="array" ref="J85">_xll.XLL.OPTION.PDF(I85, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1696,8 +2303,16 @@
         <f t="array" ref="K85">_xll.XLL.OPTION.CDF(I85, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="86" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L85" cm="1">
+        <f t="array" ref="L85">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I85, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M85" cm="1">
+        <f t="array" ref="M85">_xll.XLL.BLACK.PUT.IMPLIED(f, L85, k + I85, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J86" cm="1">
         <f t="array" ref="J86">_xll.XLL.OPTION.PDF(I86, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1706,8 +2321,16 @@
         <f t="array" ref="K86">_xll.XLL.OPTION.CDF(I86, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="87" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L86" cm="1">
+        <f t="array" ref="L86">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I86, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M86" cm="1">
+        <f t="array" ref="M86">_xll.XLL.BLACK.PUT.IMPLIED(f, L86, k + I86, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J87" cm="1">
         <f t="array" ref="J87">_xll.XLL.OPTION.PDF(I87, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1716,8 +2339,16 @@
         <f t="array" ref="K87">_xll.XLL.OPTION.CDF(I87, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="88" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L87" cm="1">
+        <f t="array" ref="L87">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I87, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M87" cm="1">
+        <f t="array" ref="M87">_xll.XLL.BLACK.PUT.IMPLIED(f, L87, k + I87, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J88" cm="1">
         <f t="array" ref="J88">_xll.XLL.OPTION.PDF(I88, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1726,8 +2357,16 @@
         <f t="array" ref="K88">_xll.XLL.OPTION.CDF(I88, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="89" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L88" cm="1">
+        <f t="array" ref="L88">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I88, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M88" cm="1">
+        <f t="array" ref="M88">_xll.XLL.BLACK.PUT.IMPLIED(f, L88, k + I88, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J89" cm="1">
         <f t="array" ref="J89">_xll.XLL.OPTION.PDF(I89, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1736,8 +2375,16 @@
         <f t="array" ref="K89">_xll.XLL.OPTION.CDF(I89, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="90" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L89" cm="1">
+        <f t="array" ref="L89">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I89, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M89" cm="1">
+        <f t="array" ref="M89">_xll.XLL.BLACK.PUT.IMPLIED(f, L89, k + I89, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J90" cm="1">
         <f t="array" ref="J90">_xll.XLL.OPTION.PDF(I90, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1746,8 +2393,16 @@
         <f t="array" ref="K90">_xll.XLL.OPTION.CDF(I90, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="91" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L90" cm="1">
+        <f t="array" ref="L90">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I90, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M90" cm="1">
+        <f t="array" ref="M90">_xll.XLL.BLACK.PUT.IMPLIED(f, L90, k + I90, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J91" cm="1">
         <f t="array" ref="J91">_xll.XLL.OPTION.PDF(I91, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1756,8 +2411,16 @@
         <f t="array" ref="K91">_xll.XLL.OPTION.CDF(I91, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="92" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L91" cm="1">
+        <f t="array" ref="L91">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I91, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M91" cm="1">
+        <f t="array" ref="M91">_xll.XLL.BLACK.PUT.IMPLIED(f, L91, k + I91, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J92" cm="1">
         <f t="array" ref="J92">_xll.XLL.OPTION.PDF(I92, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1766,8 +2429,16 @@
         <f t="array" ref="K92">_xll.XLL.OPTION.CDF(I92, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="93" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L92" cm="1">
+        <f t="array" ref="L92">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I92, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M92" cm="1">
+        <f t="array" ref="M92">_xll.XLL.BLACK.PUT.IMPLIED(f, L92, k + I92, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J93" cm="1">
         <f t="array" ref="J93">_xll.XLL.OPTION.PDF(I93, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1776,8 +2447,16 @@
         <f t="array" ref="K93">_xll.XLL.OPTION.CDF(I93, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="94" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L93" cm="1">
+        <f t="array" ref="L93">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I93, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M93" cm="1">
+        <f t="array" ref="M93">_xll.XLL.BLACK.PUT.IMPLIED(f, L93, k + I93, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J94" cm="1">
         <f t="array" ref="J94">_xll.XLL.OPTION.PDF(I94, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1786,8 +2465,16 @@
         <f t="array" ref="K94">_xll.XLL.OPTION.CDF(I94, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="95" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L94" cm="1">
+        <f t="array" ref="L94">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I94, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M94" cm="1">
+        <f t="array" ref="M94">_xll.XLL.BLACK.PUT.IMPLIED(f, L94, k + I94, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J95" cm="1">
         <f t="array" ref="J95">_xll.XLL.OPTION.PDF(I95, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1796,8 +2483,16 @@
         <f t="array" ref="K95">_xll.XLL.OPTION.CDF(I95, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="96" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L95" cm="1">
+        <f t="array" ref="L95">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I95, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M95" cm="1">
+        <f t="array" ref="M95">_xll.XLL.BLACK.PUT.IMPLIED(f, L95, k + I95, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J96" cm="1">
         <f t="array" ref="J96">_xll.XLL.OPTION.PDF(I96, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1806,8 +2501,16 @@
         <f t="array" ref="K96">_xll.XLL.OPTION.CDF(I96, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="97" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L96" cm="1">
+        <f t="array" ref="L96">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I96, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M96" cm="1">
+        <f t="array" ref="M96">_xll.XLL.BLACK.PUT.IMPLIED(f, L96, k + I96, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J97" cm="1">
         <f t="array" ref="J97">_xll.XLL.OPTION.PDF(I97, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1816,8 +2519,16 @@
         <f t="array" ref="K97">_xll.XLL.OPTION.CDF(I97, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="98" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L97" cm="1">
+        <f t="array" ref="L97">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I97, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M97" cm="1">
+        <f t="array" ref="M97">_xll.XLL.BLACK.PUT.IMPLIED(f, L97, k + I97, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J98" cm="1">
         <f t="array" ref="J98">_xll.XLL.OPTION.PDF(I98, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1826,8 +2537,16 @@
         <f t="array" ref="K98">_xll.XLL.OPTION.CDF(I98, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="99" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L98" cm="1">
+        <f t="array" ref="L98">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I98, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M98" cm="1">
+        <f t="array" ref="M98">_xll.XLL.BLACK.PUT.IMPLIED(f, L98, k + I98, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J99" cm="1">
         <f t="array" ref="J99">_xll.XLL.OPTION.PDF(I99, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1836,8 +2555,16 @@
         <f t="array" ref="K99">_xll.XLL.OPTION.CDF(I99, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="100" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L99" cm="1">
+        <f t="array" ref="L99">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I99, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M99" cm="1">
+        <f t="array" ref="M99">_xll.XLL.BLACK.PUT.IMPLIED(f, L99, k + I99, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J100" cm="1">
         <f t="array" ref="J100">_xll.XLL.OPTION.PDF(I100, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1846,8 +2573,16 @@
         <f t="array" ref="K100">_xll.XLL.OPTION.CDF(I100, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="101" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L100" cm="1">
+        <f t="array" ref="L100">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I100, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M100" cm="1">
+        <f t="array" ref="M100">_xll.XLL.BLACK.PUT.IMPLIED(f, L100, k + I100, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J101" cm="1">
         <f t="array" ref="J101">_xll.XLL.OPTION.PDF(I101, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1856,8 +2591,16 @@
         <f t="array" ref="K101">_xll.XLL.OPTION.CDF(I101, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="102" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L101" cm="1">
+        <f t="array" ref="L101">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I101, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M101" cm="1">
+        <f t="array" ref="M101">_xll.XLL.BLACK.PUT.IMPLIED(f, L101, k + I101, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J102" cm="1">
         <f t="array" ref="J102">_xll.XLL.OPTION.PDF(I102, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1866,8 +2609,16 @@
         <f t="array" ref="K102">_xll.XLL.OPTION.CDF(I102, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="103" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L102" cm="1">
+        <f t="array" ref="L102">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I102, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M102" cm="1">
+        <f t="array" ref="M102">_xll.XLL.BLACK.PUT.IMPLIED(f, L102, k + I102, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J103" cm="1">
         <f t="array" ref="J103">_xll.XLL.OPTION.PDF(I103, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1876,8 +2627,16 @@
         <f t="array" ref="K103">_xll.XLL.OPTION.CDF(I103, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="104" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L103" cm="1">
+        <f t="array" ref="L103">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I103, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M103" cm="1">
+        <f t="array" ref="M103">_xll.XLL.BLACK.PUT.IMPLIED(f, L103, k + I103, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J104" cm="1">
         <f t="array" ref="J104">_xll.XLL.OPTION.PDF(I104, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1886,8 +2645,16 @@
         <f t="array" ref="K104">_xll.XLL.OPTION.CDF(I104, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="105" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L104" cm="1">
+        <f t="array" ref="L104">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I104, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M104" cm="1">
+        <f t="array" ref="M104">_xll.XLL.BLACK.PUT.IMPLIED(f, L104, k + I104, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J105" cm="1">
         <f t="array" ref="J105">_xll.XLL.OPTION.PDF(I105, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1896,8 +2663,16 @@
         <f t="array" ref="K105">_xll.XLL.OPTION.CDF(I105, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="106" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L105" cm="1">
+        <f t="array" ref="L105">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I105, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M105" cm="1">
+        <f t="array" ref="M105">_xll.XLL.BLACK.PUT.IMPLIED(f, L105, k + I105, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J106" cm="1">
         <f t="array" ref="J106">_xll.XLL.OPTION.PDF(I106, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1906,8 +2681,16 @@
         <f t="array" ref="K106">_xll.XLL.OPTION.CDF(I106, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="107" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L106" cm="1">
+        <f t="array" ref="L106">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I106, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M106" cm="1">
+        <f t="array" ref="M106">_xll.XLL.BLACK.PUT.IMPLIED(f, L106, k + I106, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J107" cm="1">
         <f t="array" ref="J107">_xll.XLL.OPTION.PDF(I107, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1916,8 +2699,16 @@
         <f t="array" ref="K107">_xll.XLL.OPTION.CDF(I107, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="108" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L107" cm="1">
+        <f t="array" ref="L107">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I107, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M107" cm="1">
+        <f t="array" ref="M107">_xll.XLL.BLACK.PUT.IMPLIED(f, L107, k + I107, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J108" cm="1">
         <f t="array" ref="J108">_xll.XLL.OPTION.PDF(I108, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1926,8 +2717,16 @@
         <f t="array" ref="K108">_xll.XLL.OPTION.CDF(I108, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="109" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L108" cm="1">
+        <f t="array" ref="L108">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I108, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M108" cm="1">
+        <f t="array" ref="M108">_xll.XLL.BLACK.PUT.IMPLIED(f, L108, k + I108, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J109" cm="1">
         <f t="array" ref="J109">_xll.XLL.OPTION.PDF(I109, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1936,8 +2735,16 @@
         <f t="array" ref="K109">_xll.XLL.OPTION.CDF(I109, $C$8)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="110" spans="10:11" x14ac:dyDescent="0.45">
+      <c r="L109" cm="1">
+        <f t="array" ref="L109">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I109, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M109" cm="1">
+        <f t="array" ref="M109">_xll.XLL.BLACK.PUT.IMPLIED(f, L109, k + I109, t)</f>
+        <v>9.9999999999999881E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J110" cm="1">
         <f t="array" ref="J110">_xll.XLL.OPTION.PDF(I110, $C$7)</f>
         <v>0.39894228040143265</v>
@@ -1945,6 +2752,14 @@
       <c r="K110" cm="1">
         <f t="array" ref="K110">_xll.XLL.OPTION.CDF(I110, $C$8)</f>
         <v>0.5</v>
+      </c>
+      <c r="L110" cm="1">
+        <f t="array" ref="L110">_xll.XLL.OPTION.PUT(f, sigma*SQRT(t), k + I110, $C$7)</f>
+        <v>1.9945036390476076</v>
+      </c>
+      <c r="M110" cm="1">
+        <f t="array" ref="M110">_xll.XLL.BLACK.PUT.IMPLIED(f, L110, k + I110, t)</f>
+        <v>9.9999999999999881E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1972,7 +2787,7 @@
       </c>
       <c r="E2" cm="1">
         <f t="array" ref="E2">_xll.XLL.SEQUENCE.LIST({0,0})</f>
-        <v>-58650494</v>
+        <v>28247072</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
@@ -1987,7 +2802,7 @@
       </c>
       <c r="E3" cm="1">
         <f t="array" ref="E3">_xll.XLL.SEQUENCE.CONCATENATE(E2,D7)</f>
-        <v>-58659306</v>
+        <v>29750430</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>6</v>
@@ -2039,10 +2854,10 @@
       </c>
       <c r="C7" cm="1">
         <f t="array" ref="C7">_xll.XLL.CUMULANT.POISSON(C6)</f>
-        <v>28063582</v>
+        <v>29546770</v>
       </c>
       <c r="D7">
-        <v>-23650</v>
+        <v>28155464</v>
       </c>
       <c r="G7">
         <f>MIN(_xll.XLL.SEQUENCE.TAKE(C9,G8))</f>
@@ -2055,19 +2870,19 @@
     <row r="8" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C8" cm="1">
         <f t="array" ref="C8">_xll.XLL.CUMULANT.SCALE(C7, C5)</f>
-        <v>27670150</v>
+        <v>28155584</v>
       </c>
       <c r="E8" cm="1">
         <f t="array" ref="E8">_xll.XLL.BELL.REDUCED(E3,1)</f>
-        <v>-58650728</v>
+        <v>28247342</v>
       </c>
       <c r="F8" cm="1">
         <f t="array" ref="F8">_xll.XLL.HERMITE(H3)</f>
-        <v>27986570</v>
+        <v>28593288</v>
       </c>
       <c r="G8" cm="1">
         <f t="array" ref="G8">_xll.XLL.SEQUENCE.MUL(E8,F8)</f>
-        <v>-58658340</v>
+        <v>29750094</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>7</v>

</xml_diff>